<commit_message>
changed the second pool
</commit_message>
<xml_diff>
--- a/Secondpool.xlsx
+++ b/Secondpool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minsik/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10D9E66C-3CDE-6D45-84A7-1770F66C414A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB7E46AF-080E-6D4C-8C65-86359E6F6E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37800" yWindow="1360" windowWidth="27240" windowHeight="16420" xr2:uid="{230BE79E-3FC9-FA4D-8889-E10245601C1D}"/>
+    <workbookView xWindow="34320" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{836AF62A-00A5-1946-A0E7-5D7D0C5AA3F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="1014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="1450">
   <si>
     <t>Publication Year</t>
   </si>
@@ -3078,13 +3078,1524 @@
   </si>
   <si>
     <t>Disembodied electronic sounds constitute a large part of the modern auditory lexicon, but research into timbre perception has focused mostly on the tones of conventional acoustic musical instruments. It is unclear whether insights from these studies generalize to electronic sounds, nor is it obvious how these relate to the creation of such sounds. This work presents an experiment on the semantic associations of sounds produced by FM synthesis with the aim of identifying whether existing models of timbre semantics are appropriate for such sounds. A novel experimental paradigm, in which experienced sound designers responded to semantic prompts by programming a synthesizer, was applied, and semantic ratings on the sounds they created were provided. Exploratory factor analysis revealed a five-dimensional semantic space. The first two factors mapped well to the concepts of luminance, texture, and mass. The remaining three factors did not have clear parallels, but correlation analysis with acoustic descriptors suggested an acoustical relationship to luminance and texture. The results suggest that further inquiry into the timbres of disembodied electronic sounds, their synthesis, and their semantic associations would be worthwhile and that this could benefit research into auditory perception and cognition and synthesis control and audio engineering.</t>
+  </si>
+  <si>
+    <t>Kostek, Bożena</t>
+  </si>
+  <si>
+    <t>Auditory Display From The Music Technology Perspective</t>
+  </si>
+  <si>
+    <t>This paper presents some applications of Auditory Displays (AD) in the domain of music technology. First, the scope of music technology and auditory display areas are shortly outlined. Then, the research trends and system solutions within the fields of music technology, music information retrieval and music recommendation are discussed. Finally, an example of an auditory display that facilities music annotation process based on gaze tracking is shown.</t>
+  </si>
+  <si>
+    <t>Li, Grace; Walker, Bruce N.</t>
+  </si>
+  <si>
+    <t>Mixed speech and non-speech auditory displays: impacts of design, learning, and individual differences in musical engagement</t>
+  </si>
+  <si>
+    <t>Information presented in auditory displays is often spread across multiple streams to make it easier for listeners to distinguish between different sounds and changes in multiple cues. Due to the limited resources of the auditory sense and the fact that they are often untrained compared to the visual senses, studies have tried to determine the limit to which listeners are able to monitor different auditory streams while not compromising performance in using the displays. This study investigates the difference between non-speech auditory displays, speech auditory displays, and mixed displays; and the effects of the different display designs and individual differences on performance and learnability. Results showed that practice with feedback significantly improves performance regardless of the display design and that individual differences such as active engagement in music and motivation can predict how well a listener is able to learn to use these displays. Findings of this study contribute to understanding how musical experience can be linked to usability of auditory displays, as well as the capability of humans to learn to use their auditory senses to overcome visual workload and receive important information.</t>
+  </si>
+  <si>
+    <t>Mauney, Lisa M.; Walker, Bruce N.</t>
+  </si>
+  <si>
+    <t>Individual Differences and the Field of Auditory Display: Past Research, A Present Study, and an Agenda for the Future</t>
+  </si>
+  <si>
+    <t>There has been some interest in the study of individual differences in the field of auditory displays, but we argue that there is a much greater potential than has been realized, to date. Relevant types of individual differences that may be applicable to interpreting auditory information include perceptual abilities, cognitive abilities, musical abilities, and learning styles. There are many measures of these individual differences available; however, they have not been thoroughly utilized in the auditory display arena. We discuss several types of individual differences relevant to auditory displays. We then present some examples of past research, along with the results of a current investigation of individual differences in auditory displays. Finally, we propose an agenda as to what research and tests should be used to further study this area.</t>
+  </si>
+  <si>
+    <t>Tran, Quan T.; Mynatt, Elizabeth D.</t>
+  </si>
+  <si>
+    <t>Music monitor: Dynamic data display</t>
+  </si>
+  <si>
+    <t>In this demo, we present an interface prototype of Music Monitor, an application targeted for home use that dynamically conducts music in real-time to reflect parallel activities in disparate locations (e.g., preparing food in the kitchen while entertaining guests in the living room) to help the user balance attention appropriately between them. Music Monitor interprets salient information from the monitored activities to map into simple music profiles (e.g., instrument selection, tempo). The prototype design focuses on providing continuous, ambient music as a peripheral auditory data display for the primary user without sacrificing aesthetic musical value for other participants and listeners.</t>
+  </si>
+  <si>
+    <t>Alty, James L.; Rigas, Dimitrios; Vickers, Paul</t>
+  </si>
+  <si>
+    <t>Music and speech in auditory interfaces: When is one mode more appropriate than another?</t>
+  </si>
+  <si>
+    <t>A number of experiments, which have been carried out using non-speech auditory interfaces, are reviewed and the advantages and disadvantages of each are discussed. The possible advantages of using non-speech audio media such as music are discussed – richness of the representations possible, the aesthetic appeal, and the possibilities of such interfaces being able to handle abstraction and consistency across the interface.</t>
+  </si>
+  <si>
+    <t>Won, Sook Young</t>
+  </si>
+  <si>
+    <t>Auditory display of genome data: Human chromosome 21</t>
+  </si>
+  <si>
+    <t>The motivation for this paper is to systematically explore the efficacy of mapping data to sound parameters with the specific aim of sonifying statistical trends and hearing the `gist' [1] of the data. In this paper, we consider the task of searching through a gene sequence of the human chromosome 21 for CpG islands and type of gene evidence. Musical intervals and rhythm is proposed for detecting CpG islands and musical timber is used for representing the gene evidence. We extract human genome data from the NCBI (National Center for Biotechnology Information) [2] database and use list processing and synthesis capabilities of CLM [3].</t>
+  </si>
+  <si>
+    <t>Neuhoff, J. G.; Knight, R.; Wayand, J.</t>
+  </si>
+  <si>
+    <t>Pitch change, sonification, and musical expertise: Which way is up?</t>
+  </si>
+  <si>
+    <t>Frequency change is one of the most widely used acoustic dimensions in auditory display, and pitch perception is among the most widely researched topics in audition. Nonetheless, there is little research on the appropriate mapping and scaling of information to acoustic frequency in sonification. Here, we show that musical training is a contributing factor to the mapping, scaling, and conceptual relationships that exist between the information to be sonified and its acoustic representation. In Experiment 1, three groups of listeners that varied in musical expertise moved a slider to indicate the amount of pitch change that they heard in ten non-standard musical intervals. Listeners with more musical training showed greater slider movement in response to pitch change than musical novices, but not in response to brightness in a visual control condition. Novices also made significantly more errors in identifying the direction of pitch change for intervals that were well above discrimination thresholds. Experiment 2 showed that the errors by novices were due primarily to conceptual errors in labeling `rising' and `falling' pitch with a small but significant number of perceptual discrimination errors. The results suggest that musical training is an important factor in the mapping, scaling, and conceptual relationships used in sonification.</t>
+  </si>
+  <si>
+    <t>Vickers, P.</t>
+  </si>
+  <si>
+    <t>External auditory representations of programs: Past, present, and future - an aesthetic perspective</t>
+  </si>
+  <si>
+    <t>This paper provides a summary of previous work done in the area of external auditory representations of programs (known as program auralisation). A brief historical review is given followed by a short summary of the characteristics of the main program auralisation systems that have been reported in the literature. As program auralisation systems tend to use musical representations they are necessarily affected by artistic considerations. The influence of art theory and practice on the design of computer systems and artefacts (known as aesthetic computing [1, 2]) has grown to the extent that there is now a growing field devoted to its study. Therefore, it is instructive to explore the design of program auralisation systems in the light of aesthetic computing ideas. The remainder of this paper then, discusses the main principles of aesthetic computing in relation to program auralisation, and finishes with some views on how aesthetic computing can influence the future development of program auralisation systems.</t>
+  </si>
+  <si>
+    <t>Hogg, B.; Vickers, P.</t>
+  </si>
+  <si>
+    <t>Sonification abstraite/sonification concrete: An 'aesthetic persepctive space' for classifying auditory displays in the ars musica domain</t>
+  </si>
+  <si>
+    <t>This paper discusses æsthetic issues of sonifications and the relationships between sonification (ars informatica) and music &amp; sound art (ars musica). It is posited that many sonifications have suffered from poor internal ecological validity which makes listening more difficult, thereby resulting in poorer data extraction and inference on the part of the listener. Lessons are drawn from the electroacoustic music and musique concrète communities as it is argued that it is not instructive to distinguish between sonifications and music/sound art. Edgard Varèse defined music as organised sound, and sonifications organise sound to reflect mimetically the thing being sonified. Therefore, an æsthetic perspective space onto which sonifications and musical compositions alike can be mapped is proposed. The resultant map allows sonifications to be compared with works in the ars musica domain with which they share characteristics. The æsthetics of those ars musica counterparts can then be interrogated revealing useful design and organisation constructs that can be used to improve the sonifications' communicative ability.</t>
+  </si>
+  <si>
+    <t>Joseph, A. J.; Lodha, S. K.</t>
+  </si>
+  <si>
+    <t>Musart: Musical audio transfer function real-time toolkit</t>
+  </si>
+  <si>
+    <t>This work describes the design and implementation of a sonification toolkit. MUSART (MUSical Audio transfer function Realtime Toolkit) is a sonification toolkit which produces musical sound maps that are played in real-time. Register, pitch, timbre, chords, duration, silence, loudness, beats, and panning are the musical concepts used to create melodic sound maps. Univariate and multivariate data sets are sonified using various sound parameter combinations and music tracks. Users have the flexibility to create personalized auditory displays by mapping each data dimension of a data set to one or more sound parameters. MUSART is designed to be flexible so that it can be used with many applications. In this work, we use musical auditory maps to explore seismic volumes used for detecting areas for drilling oil.</t>
+  </si>
+  <si>
+    <t>Fagerlon, Johan</t>
+  </si>
+  <si>
+    <t>Expressive Musical Warning Signs</t>
+  </si>
+  <si>
+    <t>Warning signals are often very simple and monotone sounds. This paper focuses on taking a more musical approach to the design of warnings and alarms than has been the case in the past. We present an experimental pilot study in which we explore the possibilities of using short musical pieces as warning signals in a vehicle cab. In the study, 18 experienced drivers experienced five different driving scenarios with different levels of urgency. Each scenario was presented together with an auditory icon, a traditional abstract warning sound, and a musical warning sound designed in collaboration with a composer. The test was carried out in an “audio-only” environment. Drivers were required to rate the perceived urgency, annoyance and appropriateness for every sound. They also had a chance to talk freely about the different warning signals. The results indicate interestingly that drivers may be able to understand the intended meaning of musical warning signals. It seems like the musical warning signals may prove useful primarily in situations of low and medium levels of urgency.</t>
+  </si>
+  <si>
+    <t>Winters, R. Michael</t>
+  </si>
+  <si>
+    <t>1/F Noise and Auditory Aesthetics: Sonification of a Driven Bead Pile</t>
+  </si>
+  <si>
+    <t>“1=f noise” describes the behavior of many naturally occurring complex dynamical systems over time. Perhaps more surprising than its ubiquity in nature is its prevalence in speech and especially music. Current research suggests that aspects of the human emotional response to music can be predicted using analysis based upon 1=f distributions. Musical compositions in which the pitch and duration of notes over time correspond to 1=f distributions have been found to be more pleasant than non-1=f distributions. The current research compares the sonification of a driven bead pile to an experimentally contrived deviation. Preliminary results suggest that the findings of pitch and duration may be extended to timbre and spatialization. The benefits of continued research into the application 1=f distributions in sonification for the auditory display community are discussed.</t>
+  </si>
+  <si>
+    <t>Childs, Edward</t>
+  </si>
+  <si>
+    <t>Auditory graphs of real-time data</t>
+  </si>
+  <si>
+    <t>The advantages of auditory display for monitoring real-time data are discussed. Parallels between the structures of real-time data and music are emphasized as potentially fruitful areas of research. The Accentus LLC design philosophy is described, followed by several examples of auditory graphs. Areas of future research are recommended.</t>
+  </si>
+  <si>
+    <t>Tislar, Kay; Duford, Zackery; Nelson, Brittany; Peabody, Madeline; Jeon, Myounghoon</t>
+  </si>
+  <si>
+    <t>Examining the learnability of auditory displays: Music, earcons, spearcons, and lyricons</t>
+  </si>
+  <si>
+    <t>Auditory displays are a useful platform to convey information to users for a variety of reasons. The present study sought to examine the use of different types of sounds that can be used in auditory displays—music, earcons, spearcons, and lyricons—to determine which sounds have the highest learnability when presented in sequences. Participants were self-trained on sound meanings and then asked to recall meanings after listening to sequences of varying lengths. The relatedness of sounds and their attributed meanings, or the intuitiveness of the sounds, was also examined. The results show that participants were able to learn and recall lyricons and spearcons the best, and related meaning is an important contributing variable to learnability and memorability of all sound types. This should open the door for future research and experimentation of lyricons and spearcons presented in auditory streams.</t>
+  </si>
+  <si>
+    <t>New Directions for Sonification of Expressive Movement in Music</t>
+  </si>
+  <si>
+    <t>Expert musical performance is rich with visual cues that facilitate expressive communication. Previous sonifications in this domain have evaluated the saliency of mapping based upon a sound's direct visual correspondence. Although this approach may be important for motion sonification more generally, a little flexibility might be necessary for expressive gesture. A review of literature on gesture in music performance suggests that for evaluation, it matters less what is moving than how and how much. New efforts focus on the potential use of sonification with the underlying performance audio. A series of videos and sonifications are presented as examples of this point.</t>
+  </si>
+  <si>
+    <t>Gossmann, Joachim</t>
+  </si>
+  <si>
+    <t>Towards an auditory representation of complexity</t>
+  </si>
+  <si>
+    <t>In applications of sonification, the information inferred by the sonification strategy applied often supersedes the amount of information which can be retrieved by the ear about the object of sonification. This paper focuses on the representation of complex geometric formation through sound, drawing on the development of an interactive installation sonifying escape time fractals as an example. The terms “auditory emergence and formation” are introduced and an attempt is made to interpret them for music composition, data display and information theory. The example application,. “Audio Fraktal”, is a public installation in the permanent exhibition of the Museum for Media Art at ZKM, Karlsruhe. The design of the audiovisual display system that allows the shared experience of interactive spatial auditory formation is described. The work was produced by the author at the Institute for Music and Acoustics at ZKM, Karlsruhe.</t>
+  </si>
+  <si>
+    <t>Preti, Constanza; Schubert, Emery</t>
+  </si>
+  <si>
+    <t>Sonification of Emotions II: Live music in a pediatric hospital</t>
+  </si>
+  <si>
+    <t>In this paper, we argue that music can be used to sonify emotions. Further, we propose that the ‘sonification of emotion’ conceptualization can explain some aspects of the practice of playing music in hospitals. Music can be constantly adjusted to reflect (but more accurately, we argue, sonify) various aspects of the emotional situations unfolding in a hospital, namely the interaction between the child/patient, their caregivers and the hospital staff. The case study of a musical interaction between a musician and a child/patient is presented and led to the development of a Cycle of Sonification model, where the musician collects complex environmental cues and then portrays them through the music to adjust the emotional ‘temperature’. That is, the emotion of the environment is reflected (sonified) by the music, but additionally the music is also calibrated so as to allow the regulation of the emotional mood (including distraction) in the otherwise stressful environment. As well as adjusting the mood, the music provides a ‘reading’ or measure of emotion through the auditory, non-speech mode, consistent with some pertinent definitions of sonification</t>
+  </si>
+  <si>
+    <t>Lodha, Suresh K.; Beahan, John; Heppe, Travis; Joseph, Abigail; Zane-Ulman, Brett</t>
+  </si>
+  <si>
+    <t>MUSE: A musical data sonification toolkit</t>
+  </si>
+  <si>
+    <t>Data sonification is the representation of data using sound. Last year we presented a flexible, interactive and portable data sonification toolkit called LISTEN, that allows mapping of data to several sound parameters such as pitch, volume, timbre and duration [20]. One of the potential drawbacks of LISTEN is that since the sounds generated are non-musical, they can be fatiguing when exploring large data sets over extended periods of time. A primary goal in the design of MUSE – a MUsical Sonification Environment – is to map scientific data to musical sounds. The challenge is to ensure that the data meanings are preserved and brought out by these mappings. MUSE provides flexible data mappings to musical sounds using parameters such as pitch (melody), rhythm, tempo, volume, timbre and harmony. MUSE is written in C++ for the SGI platform and works with the freely available sound specification software CSound developed at MIT. We have applied MUSE to map uncertainty in some scientific data sets to musical sounds.</t>
+  </si>
+  <si>
+    <t>Straebel, Volker</t>
+  </si>
+  <si>
+    <t>The Sonification Metaphor in Instrumental Music and Sonification's Romantic Implications</t>
+  </si>
+  <si>
+    <t>Vickers, Paul; Alty, James L.</t>
+  </si>
+  <si>
+    <t>CAITLIN: A musical problem auralisation tool to assist novice programmers with debugging</t>
+  </si>
+  <si>
+    <t>In the field of auditory display relatively little work has focused on the use of sound to aid program debugging. In this paper, we describe CAITLIN , a pre-processor for Turbo Pascal programs that musically auralises programs with a view to assisting novice programmers with locating errors in their code. A discussion follows of an experiment which showed that programmers could use the musical feedback to visualise and describe program structure. We then present conclusions and a discussion of future work.</t>
+  </si>
+  <si>
+    <t>Ash, Kingsley</t>
+  </si>
+  <si>
+    <t>Affected States: Analysis and Sonification of Twitter Music Trends</t>
+  </si>
+  <si>
+    <t>This paper describes an approach to the sonification of real- time twitter music trend data realized for the ICAD 2012 Sonification Competition: Listening to the World Listening. The paper will discuss the techniques used to create the sonification and the motivations behind them, including details of the data analysis, mapping strategies, visual display and sonification output. The system analyses the Twitter Music Trends data feed, which aggregates music listening data from Twitter by artist, as well as the Echo Nest REST API to determine the perceived emotional affect and prevailing descriptions of a selection of the latest trending artists. The resulting data is visualized and sonified in real-time to facilitate analysis and generate an appealing visual and auditory display of the resulting data. Experience with the system suggests that it is successful in allowing users to determine perceived emotional affect and quality for a number of artists simultaneously, and could allow further investigation into the correlation between these factors. The system also generates appealing visual music that reaches beyond the practice of scientific investigation to reach out to a wider audience.</t>
+  </si>
+  <si>
+    <t>Ocean buoy spectral data sonification: Research update</t>
+  </si>
+  <si>
+    <t>Since first presenting this work at the 2002 International Conference on Auditory Display the author has professionally produced a multimedia CD that explores the sonification of ocean wave data. “Music from the Ocean” is a multimedia CD that explores the sonification of ocean wave data for oceanography, science pedagogy, and music and sound synthesis. Turning this data into sound provides new ways of experiencing and comprehending the phenomena involved; the processes come alive and are more comprehensible, memorable and exciting than graphs of the data. This CD contains over 55 minutes of sound examples as well as an interactive Flash presentation and research paper explaining the methods in more detail. The accompanying 16-page booklet features graphics and information about the data, phenomena, and music. The CD appeals to a wide variety of consumers, from oceanographers, science teachers, experimental computer music enthusiasts, and music therapists.</t>
+  </si>
+  <si>
+    <t>Oswald, David</t>
+  </si>
+  <si>
+    <t>Non-Speech Audio-Semiotics: A Review and Revision of Auditory Icon and Earcon Theory</t>
+  </si>
+  <si>
+    <t>The aim of this paper is to develop a theory and taxonomy of auditory signs, based on semiotics. For more than two decades, the discourse on non-speech audio interfaces has been dominated by a dichotomy between auditory icons, which are based on everyday hearing, and earcons, which are based on musical hearing. The corresponding theory behind these concepts has to be revised for several reasons. First, the authors of these theories partly use semiotic concepts and terminology, but not always in a correct way. Second, the classification of auditory icons as "iconic", and earcons as "abstract" is too simple and based on the questionable premise that everyday sounds are per se iconic and musical motives are per se abstract and symbolic. Third, this widespread idea ignores the crucial role of the user in the process of perception. In addition, the users' perception of visual and auditory signs in computer interfaces is fundamentally different today, from how it was in the early years of graphical user interfaces — the time when the first auditory interfaces and the corresponding theories were developed.</t>
+  </si>
+  <si>
+    <t>Schubert, Emery; Ferguson, Sam; Farrar, Natasha; McPherson, Gary E.</t>
+  </si>
+  <si>
+    <t>Sonification of Emotion I: Film Music</t>
+  </si>
+  <si>
+    <t>This paper discusses the uses of sound to provide information about emotion. The review of the literature suggests that music is able to communicate and express a wide variety of emotions. The novel aspect of the present study is a reconceptualisation of this literature by considering music as having the capacity to sonify emotions. A study was conducted in which excerpts of non-vocal film music were selected to sonify six putative emotions. Participants were then invited to identify which emotions each excerpt sonified. The results demonstrate a good specificity of emotion sonification, with errors attributable to selection of emotions close in meaning to the target (excited confused with happy, but not with sad, for example). While ‘sonification’ of emotions has been applied in opera and film for some time, the present study allows a new way of conceptualizing the ability of sound to communicate affect through music. Philosophical and psychological implications are considered.</t>
+  </si>
+  <si>
+    <t>Margounakis, D.; Politis, D.</t>
+  </si>
+  <si>
+    <t>Converting images to music using their colour properties</t>
+  </si>
+  <si>
+    <t>Music is associated to colors since ancient years. Different mappings between attributes of sound and images allow the efficient conversion between the two types of media. The proposed method for converting images to music using the concept of chromaticism provides the area of computer music with a parameterized environment for audio-visual presentations. The auditory display of colour images may bring the different ways that a listener perceives a musical piece (because of colour transitions) to light. A design template for chromatic synthesis is described. A short example, based on a graphical digital icon, demonstrates the preliminary results.</t>
+  </si>
+  <si>
+    <t>Understanding The Need For Micro-Gestural Inflections In Parameter-Mapping Sonification</t>
+  </si>
+  <si>
+    <t>Most of the software tools used for data sonification have been adopted or adapted from those designed to compose computer music, which in turn, adopted them from abstractly notated scores. Such adoptions are not value-free; by using them, the cultural paradigms underlying the music for which the tools were made have influenced the conceptualization and, it is argued, the effectiveness of data sonifications. Recent research in cognition supports studies in empirical musicology that suggest that listening is not a passive ingestion of organised sounds but is an embodied activity that invisibly enacts gestures of what is heard. This paper outlines an argument for why sonifiers using parametric-mapping sonification should consider incorporating micro-gestural inflections if they are to mitigate The Mapping Problem in enhancing the intelligibility of sonified data.</t>
+  </si>
+  <si>
+    <t>Jung, Ralf</t>
+  </si>
+  <si>
+    <t>Ambience for Auditory Displays: Embedded Musical Instruments As Peripheral Audio Cues</t>
+  </si>
+  <si>
+    <t>From alarm signals and data sonification to multimodal interfaces, auditory displays are omnipresent in our everyday life and they become more and more popular. But there are some challenges we have to meet because of the differentness of the auditory sense compared to the visual sense. Usually, audio notification signals are limited to simple warning cues and system feedback that are in most cases intrusive be- cause they differ from the environmental noise. That has the effect that people present in the room could be distracted from their current tasks because they cannot “close their ears.” To prevent the disturbing effect of traditional notification signals we developed the novel concept of non-speech audio notification embedded in ambient soundscapes to provide multi-user notification in a more discreet and non-disturbing way. Instead of using well-known non-speech cues like auditory icons and earcons, we decided to compose and record peripheral soundscapes and notification instruments by ourselves towards a more aesthetic approach. In this paper, we give an overview of our location-aware system with two applications (PAAN, AeMN) and sketch a real life scenario in a wine department of a supermarket. We will also present findings from a user study and provide a small collection of notification instruments and soundscapes as audio samples.</t>
+  </si>
+  <si>
+    <t>Schmele, Timothy; Gomez, Imanol</t>
+  </si>
+  <si>
+    <t>Exploring 3D audio for brain sonification</t>
+  </si>
+  <si>
+    <t>Brain activity data, measured by functional Magnetic Resonance Imaging (fMRI), produces extremely high dimensional, sparse and noisy signals which are difficult to visualize, monitor and analyze. The use of spatial music can be particularly appropriate to represent its contained patterns. The literature describes several research done on sonifying neuroimaging data as well as different techniques to use spatialization as a musical language. In this paper, we discuss an artistic approach to fMRI sonification exploiting new compositional paradigms in spatial music. There fore, we have consider the brain activity as audio base material of a the spatial musical composition. Our approach attempts to explore the aesthetic potential of brain sonification not by transforming the data beyond the recognizable, and presenting the data as direct as possible.</t>
+  </si>
+  <si>
+    <t>Spondike, David</t>
+  </si>
+  <si>
+    <t>A Strategy for Composing Music using the Sonification of "Snapshot" type Data Collections "Schnappschuss von der Erde"</t>
+  </si>
+  <si>
+    <t>Transforming the sonification of data into a musical experience that is satisfying on scientific as well as aesthetic grounds requires balancing similar and competing objectives and sensibilities. One possible solution, described here, is used to create the digital music composition Schnappschuss von der Erde in response to the call for compositions by the International Community for Auditory Display (ICAD) Conference.</t>
+  </si>
+  <si>
+    <t>Rönnberg, Niklas; Löwgren, Jonas</t>
+  </si>
+  <si>
+    <t>Photone: Exploring modal synergy in photographic images and music</t>
+  </si>
+  <si>
+    <t>We present Photone, an interactive installation combining photographic images and musical sonification. An image is displayed, and a dynamic musical score is generated based on the overall color properties of the image and the color value of the pixel under the cursor. Hence, the music changes as the user moves the cursor. This simple approach turns out to have interesting experiential qualities in use. The composition of images and music invites the user to explore the combination of hues and textures, and musical sounds. We characterize the resulting experience in Photone as one of modal synergy where visual and auditory output combine holistically with the chosen interaction technique. This tentative finding is potentially relevant to further research in auditory displays and multimodal interaction.</t>
+  </si>
+  <si>
+    <t>A perspective on the limited potential for simultaneity in auditory display</t>
+  </si>
+  <si>
+    <t>The auditory environment is frequently described as a juxtaposition between an array of pre-disclosed auditory streams and a process of attentional selection. The orientation of attentional selection toward environmental streams is characterized by a differentiation in the types of stream: Speech, music and sound effects are only three examples in an open polymorphism of what could be described as perceptual strategies through which we access the sounding world. The differentiable-simultaneous manifold of environmental streams allows perceptual participation only in a certain number of streams at the same time - only one speaking voice, one sense of "harmony", a single "rhythm", and so forth: We propose a re-basing of sonfication strategies not on the definition of external mechanisms, but on the definition and application of new modal strategies that are circumscribed and accessible through 'what is not possible to perceive at the same time'.</t>
+  </si>
+  <si>
+    <t>Vigani, Andrea</t>
+  </si>
+  <si>
+    <t>Sonic Window #1 [2011] — A Real Time Sonification</t>
+  </si>
+  <si>
+    <t>This is a real time audio installation in Max/MSP. It is a sonification of an abstract process: the writing on Twitter about music listening experiences on the web by people around the world. My purpose is not to sonify the effects of this process on a musical structure (the musical structure of the listened songs) like a real-time-echo-web-mix or a new version of J.Cage “Imaginary landscape n°4”, but to sonify the structure of the process itself, with its languages transducers, its media, its rules. For this purpose I created a musical instrument played by the data, like a windchimes but here all the sounds are created by the web data itself, like if the material of a windchimes is the wind itself.It’s like an open windows on the web listeners, you observe the action of listening and talking about music, but you don’t hear the music listened and you search for connections, reactions, interactions among the listeners, among them, the transmission media and the code language.</t>
+  </si>
+  <si>
+    <t>Schoon, Andi; Dombois, Florian</t>
+  </si>
+  <si>
+    <t>Sonification in Music</t>
+  </si>
+  <si>
+    <t>Seen from the vantage point of cultural history, contemporary sonification is essentially characterised by two aspects that to date have seldom been considered in combination: the first aspect is sonification as the transformation of the inaudible into the sphere of the audible, and the second its use as an instrument for gaining knowledge via the concrete listening experience. One of the aims of the research project “Denkgeräusche” ("Sounds of Thought"), conducted at Bern University of the Arts, was to make a contribution to a (yet unwritten) cultural history of sonification. With this target in mind, a database was compiled of historical and contemporary musical compositions in which procedures associated with sonification were employed.</t>
+  </si>
+  <si>
+    <t>Pape, Daniel</t>
+  </si>
+  <si>
+    <t>Is pitch perception and discrimination of vowels language-dependent and influencd by the vowels spectral properties?</t>
+  </si>
+  <si>
+    <t>Pitch discrimination and accuracy has been found to depend on different factors. However, little work has been done (1) on the cross-linguistic influence of the listeners' native language and (2) on the influence of the spectral structure on the pitch perception of vowels as well as (3) cross-linguistic differences regarding different levels of muscial education. If differences in pitch discrimination between different language families exist this would be a crucial knowledge in the design and failure-safe application of auditory displays driven by pitch differences in speech control. Therefore the current study examines pitch discrimination of German vowels with a similar vowel height differing in rounding and tenseness for (1) native German listeners and (2) native Catalan listeners. Significant differences in the sensitivity of pitch perception between these two languages were found. Catalan listeners, independent of their musical education, were mostly insensitive to even large pitch differences in the vowels to be judged. The accuracy of pitch judgements for German listeners were significantly different for musically educated listeners in comparison to musically uneducated listeners. Further, both languages show a significant pitch difference for rounded vowels compared to the unrounded vowels. The current study provides evidence that pitch discrimination is language-dependent, at least partially.</t>
+  </si>
+  <si>
+    <t>Andreopoulou, Areti; Goudarzi, Visda</t>
+  </si>
+  <si>
+    <t>Reflections on the Representation of Women in the International Conferences on Auditory Displays (ICAD)</t>
+  </si>
+  <si>
+    <t>This paper investigates the representation of women researchers and artists in the conferences of the International Community for Auditory Display (ICAD). In the absence of an organized membership mechanism and / or publicly available records of conference attendees, this topic was approached through the study of publication and authorship patterns of female researchers in ICAD conferences. Temporal analysis showed that, even though there has been an increase in the number of publications co-authored by female researchers, the annual percentage of female authors remained in relatively unchanged levels (mean = 17.9%) throughout the history of ICAD conferences. This level, even though low, remains within the reported percentages of female representation in other communities with related disciplines, such as the International Computer Music Association (ICMA) and the Conferences of the International Society for Music Information Retrieval (ISMIR), and significantly higher than in more audio engineering-related communities, such as the Audio Engineering Society (AES).</t>
+  </si>
+  <si>
+    <t>Jeon, Myounghoon; Sun, Yuanjing</t>
+  </si>
+  <si>
+    <t>Design and Evaluation of Lyricons (Lyrics + Earcons) for Semantic and Aesthetic Improvements of Auditory Cues</t>
+  </si>
+  <si>
+    <t>Auditory researchers have developed various non-speech cues in designing auditory user interfaces. A preliminary study of “Lyricons” (lyrics + earcons) has provided a novel approach to devising auditory cues in electronic products, by combining the concurrent two layers of musical speech and earcons (short musical motives). The purpose of the present study is to introduce iterative design processes and to validate the effectiveness of lyricons compared to earcons, whether people can more intuitively grasp functions that lyricons imply than those of earcons. Results favor lyricons over earcons. Future work and practical application directions are also discussed.</t>
+  </si>
+  <si>
+    <t>Middleton, Jonathan; Hakulinen, Jaakko; Tiitinen, Katariina; Hella, Juhu; Keskinen, Tuuli; Huuskonen, Pertti; Linna, Juhani; Turunen, Markku; Ziat, Mounia; Raisamo, Roope</t>
+  </si>
+  <si>
+    <t>Sonification with musical characteristics: a path guided by user engagement</t>
+  </si>
+  <si>
+    <t>Sonification with musical characteristics can engage users, and this dynamic carries value as a mediator between data and human perception, analysis, and interpretation. A user engagement study has been designed to measure engagement levels from conditions within primarily melodic, rhythmic, and chordal contexts. This paper reports findings from the melodic portion of the study, and states the challenges of using musical characteristics in sonifications via the perspective of form and function – a long standing debate in Human-Computer Interaction. These results can guide the design of more complex sonifications of multivariable data suitable for real life use.</t>
+  </si>
+  <si>
+    <t>Avissar, Daniel; Leider, Colby; Bennett, Hristopher; Gailey, Robert</t>
+  </si>
+  <si>
+    <t>An audio game app using interactive Movement sonification for Targeted posture control</t>
+  </si>
+  <si>
+    <t>Interactive movement sonification has been gaining validity as a technique for biofeedback and auditory data mining in research and development for gaming, sports, and physiotherapy. Naturally, the harvesting of kinematic data over recent years has been a function of an increased availability of more portable, high-precision sensory technologies, such as smart phones, and dynamic real time programming environments, such as Max/MSP. Whereas the overlap of motor skill coordination and acoustic events has been a staple to musical pedagogy, musicians and music engineers have been surprisingly less involved than biomechanical, electrical, and computer engineers in research efforts in these fields. Thus, this paper proposes a prototype for an accessible virtual gaming interface that uses music and pitch training as positive reinforcement in the accomplishment of target postures.</t>
+  </si>
+  <si>
+    <t>Evaluating the use of sonification and music to support the communication of alcohol health risk to young people: Initial results</t>
+  </si>
+  <si>
+    <t>The interdisciplinary research project, Using Sonification to COmmunicate public health Risk data (SCORe), aims to experimentally test how sonification, interactivity in combination with music, could increase the communicative potential of a visual presentation directed to young people and focused on health risk data of alcohol consumption. Specifically, we are studying how this type of presentation can support engagement with health information, and the effective interpretation and recall of data. In order to explore the possible influence of sound in understanding important health risk messages, a 3-arm pilot randomised control (participant-blinded) trial was designed. We compared a visual presentation augmented by sonification, music and interaction with a simple visual presentation and a visual presentation augmented by simple user interaction. This paper describes the most complex of the three health presentations (the audio-visual and interactive presentation) and presents initial findings that relate to this presentation only.</t>
+  </si>
+  <si>
+    <t>Polotti, Pietro; Benzi, Carlo</t>
+  </si>
+  <si>
+    <t>Rhetorical Schemes for Audio Communication</t>
+  </si>
+  <si>
+    <t>The application of rhetorical techniques to the use of non-verbal sound in the interaction between humans and technologies is the core idea of this paper. We present our ideas at a general level and illustrate an exploratory case based on the application of rhetorical schemes to the sonification of computer operating system events. Both cases of musical sounds and everyday sounds are investigated. This work is intended as a preliminary study aiming at motivating a larger scale and more rigorous research about the potentiality of the use of rhetoric in the domain of Auditory Display (AD) and Sonic Interaction Design (SID).</t>
+  </si>
+  <si>
+    <t>Quinn, Marty; Quinn, Wendy; Hatcher, Ben</t>
+  </si>
+  <si>
+    <t>For those who died: A 9/11 tribute</t>
+  </si>
+  <si>
+    <t>For Those Who Died is a 6-minute dance and music tribute to those who died on 9/11. It premiered 9/11/2002 as part of a larger event entitled “Reflections, A Gift to the Community” that occurred at the Music Hall in Portsmouth NH. It features extensive textual sonification, dance, and two layers of visual presentation of nine textual datasets containing the names of those who died on September 11, 2001, the US Constitution and some DNA from chromosomes 1 and 9. The music was produced using five Yamaha QY70 and QY100 synthesizers and presented in surround sound.</t>
+  </si>
+  <si>
+    <t>Neuhoff, John G.</t>
+  </si>
+  <si>
+    <t>Is sonification doomed to fail?</t>
+  </si>
+  <si>
+    <t>Despite persistent research and design efforts over the last twenty years, widespread adoption of sonification to display complex data has largely failed to materialize, and many of the challenges to successful sonification identified in the past persist. Major impediments to the widespread adoption sonification include fundamental perceptual differences between vision and audition, large individual differences in auditory perception, musical biases of sonification researchers, and the interdisciplinary nature of sonification research and design. The historical and often indiscriminate mingling of art and science in sonification design may be a root cause of some of these challenges. Future sonification design efforts that explicitly strive to meet either artistic or scientific goals may lead to greater clarity and success in the field and more widespread adoption of useful sonification techniques.</t>
+  </si>
+  <si>
+    <t>Winters, R. Michael; Weinberg, Gil</t>
+  </si>
+  <si>
+    <t>Sonification of the Tohoku earthquake: Music, popularization &amp; the auditory sublime</t>
+  </si>
+  <si>
+    <t>The past century has witnessed the emergence of expressive musical forms that originate in appropriated technologies and practices. In most cases, this appropriation is performed without protest— but not always. Carefully negotiating a space for sound as an objective, scientific medium, the field of sonification has cautiously guarded the term from subjective and affective endeavors. This paper explores the tensions arising in sonification popularization through a formal analysis of Sonification of the Tohoku Earthquake, a two-minute YouTube video that combined audification with a time-aligned seismograph, text and heatmap. Although the many views the video has received speak to a high public impact, the features contributing to this popularity have not been formalized, nor the extent to which these characteristics further sonifications’ scientific mission. For this purpose, a theory of popularization based upon “sublime listening experiences” is applied. The paper concludes by drawing attention to broader themes in the history of music and technology and presents guidelines for designing effective public-facing examples.</t>
+  </si>
+  <si>
+    <t>Tkaczevski, Alejandro</t>
+  </si>
+  <si>
+    <t>Auditory interface problems and solutions for commercial multimedia products</t>
+  </si>
+  <si>
+    <t>This paper will explore the various aesthetic, technical, and musical issues that sound designers face when creating audio for commercial products. I will draw from my experience at and use materials from Broderbund Software. In the first section, I will discuss issues concerning interface sonification. In the second section, I will briefly illustrate a quick musical solution to a potentially large logistical problem. In the last section, I will show a solution for balancing digital audio and MIDI on a variety of devices, drivers, and operation systems.</t>
+  </si>
+  <si>
+    <t>Kleinberger, Rebecca; George, Stefanakis; Franjou, Sebastian</t>
+  </si>
+  <si>
+    <t>Speech companions: Evaluating the effects of musically modulated auditory feedback on the voice</t>
+  </si>
+  <si>
+    <r>
+      <t>Changing the way one hears one's own voice, for instance by adding delay or shifting the pitch in real-time, can alter vocal qualities such as speed, pitch contour, or articulation. We created new types of auditory feedback called Speech Companions that generate live musical accompaniment to the spoken voice. Our system generates harmonized chorus effects layered on top of the speaker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>s voice that change chord at each pseudo-beat detected in the spoken voice. The harmonization variations follow predetermined chord progressions. For the purpose of this study we generated two versions: one following a major chord progression and the other one following a minor chord progression. We conducted an evaluation of the effects of the feedback on speakers and we present initial findings assessing how different musical modulations might potentially affect the emotions and mental state of the speaker as well as semantic content of speech, and musical vocal parameters.</t>
+    </r>
+  </si>
+  <si>
+    <t>Diniz, Nuno; Deweppe, Alexander; Demey, Michiel; Leman, Marc</t>
+  </si>
+  <si>
+    <t>A Framework for Music-based Interactive Sonification</t>
+  </si>
+  <si>
+    <t>In this paper, a framework for interactive sonification is introduced. It is argued that electroacoustic composition techniques can provide a methodology for structuring and presenting multivariable data through sound. Furthermore, an embodied music cognition driven interface is applied to provide an interactive exploration of the generated music-based output. The motivation and theoretical foundation for this work are presented as well as the framework’s implementation and an exploratory use case.</t>
+  </si>
+  <si>
+    <t>Henry, Ashley G.; Bruce, Carrie M.; Winton, Riley J.; Walker, Bruce N.</t>
+  </si>
+  <si>
+    <t>Sonification Mapping Configurations: Pairings Of Real-Time Exhibits And Sound</t>
+  </si>
+  <si>
+    <t>Visitors to aquariums typically rely on their vision to interact with live exhibits that convey rich descriptive and aesthetic visual information. However, some visitors may prefer or need to have an alternative interpretation of the exhibitÕs visual scene to improve their experience. Musical sonification has been explored as an interpretive strategy for this purpose and related work provides some guidance for sonification design, yet more empirical work on developing and validating the music-to-visual scene mappings needs to be completed. This paper discusses work to validate mappings that were developed through an investigation of musician performances for two specific live animal exhibits at the Georgia Aquarium. In this proposed study, participants will provide feedback on musical mapping examples which will help inform design of a real-time sonification system for aquarium exhibits. Here, we describe our motivation, methods, and expected contributions.</t>
+  </si>
+  <si>
+    <t>The design of a smart city sonification system using a conceptual blending and musical framework, web audio and deep learning techniques</t>
+  </si>
+  <si>
+    <t>This paper describes an auditory display system for smart city data for Dublin City, Ireland. It introduces and describes the different layers of the system and outlines how they operate individually and interact with one another. The system uses a deep learning model called a variational autoencoder to generate musical content to represent data points. Further data-to-sound mappings are introduced via parameter mapping sonification techniques during sound synthesis and post-processing. Conceptual blending and music theory provide frameworks, which govern the design of the system. The paper ends with a discussion of the design process that contextualizes the contribution, highlighting the interdisciplinary nature of the project, which spans data analytics, music composition and human-computer interaction.</t>
+  </si>
+  <si>
+    <t>Leonard, Neil</t>
+  </si>
+  <si>
+    <t>Sonification: Celestial Data and Poetic Inquiry</t>
+  </si>
+  <si>
+    <t>This paper describes a composition/sonification project to be realized by faculty and students from the Electronic Production and Design department (EP/D) at Berklee College of Music in Boston. The goal of the project is compose music for a 30- minute interdisciplinary-networked performance to be premiered in Boston, Lyon and Havana involving artists from each city. In the process, artists are examining new modes of expression and the construction of knowledge and artistic dialog. Kelly Snook, Ph.D. Astrophysicist, Division of Solar System Exploration, NASA Goddard Spaceflight Center is working with the group to choose scientific data for sonification including compelling new planetary science and solar system data.</t>
+  </si>
+  <si>
+    <t>Fox, K. Michael; Stewart, Jeremy; Hamilton, Rob</t>
+  </si>
+  <si>
+    <t>madBPM: Musical and Auditory Display for Biological Predictive Modeling</t>
+  </si>
+  <si>
+    <t>The modeling of biological data can be carried out using structured sound and musical process in conjunction with integrated visualizations. With a future goal of improving the speed and accuracy of techniques currently in use for the production of synthetic high value chemicals through the greater understanding of data sets, the madBPM project couples real-time audio synthesis and visual rendering with a highly flexible data-ingestion engine. Each component of the madBPM system is modular, allowing for customization of audio, visual and data-based processing.</t>
+  </si>
+  <si>
+    <t>Landry, Steven; Sun, Yuangjing; Slade, Darnishia; Jeon, Myounghoon</t>
+  </si>
+  <si>
+    <t>Tempo-Fit Heart Rate App: Using Heart Rate Sonification As Exercise Performance Feedback</t>
+  </si>
+  <si>
+    <t>Physical inactivity is a worldwide issue causing a variety of health problems. Exploring novel ways to encourage people to engage in physical activity is a topic at the forefront of research for countless stakeholders. Based upon a review of the literature, a pilot study, and exit interviews, we propose an app prototype that utilizes music tempo manipulation to guide users into a target heart rate zone during an exercise session. A study was conducted with 26 participants in a fifteen-minute cycling session using different sonification mappings and combinations of audiovisual feedback based on the user's current heart rate. Results suggest manipulating the playback speed of music in real time based on heart rate zone departures can be an effective motivational tool for increasing or decreasing activity levels of the listener. Participants vastly preferred prescriptive sonifications mappings over descriptive mappings, due to people's natural inclination to follow the tempo of music.</t>
+  </si>
+  <si>
+    <t>Mealla, Sebastian; Bosi, Mathieu; Jorda, Sergi; Valjamae, Aleksander</t>
+  </si>
+  <si>
+    <t>Sonification of Brain and Body Signals in Collaborative Tasks Using a Tabletop Musical Interface</t>
+  </si>
+  <si>
+    <t>Physiological Computing has been applied in different disciplines, and is becoming popular and widespread in Human-Computer In- teraction, due to device miniaturization and improvements in real- time processing. However, most of the studies on physiology- based interfaces focus on single-user systems, while their use in Computer-Supported Collaborative Work (CSCW) is still emerg- ing. The present work explores how sonification of human brain and body signals can enhance user experience in collaborative mu- sic composition. For this task, a novel multimodal interactive sys- tem is built using a musical tabletop interface (Reactable) and a hybrid Brain-Computer Interface (BCI). The described system al- lows performers to generate and control sounds using their own or their fellow team member’s physiology. Recently, we assessed this physiology-based collaboration system in a pilot experiment. Dis- cussion on the results and future work on new sonifications will be accompanied by practical demonstration during the conference.</t>
+  </si>
+  <si>
+    <t>Tissberger, Johann P.; Wersenyi, Gyorgy</t>
+  </si>
+  <si>
+    <t>Sonification Solutions for Body Movements in Rehabilitation of Locomotor Disorders</t>
+  </si>
+  <si>
+    <t>One of the recent fields of sonification focuses on the sonification of body movements in sports or rehabilitation. This is usually some kind of monitoring of real-time measurement data and auditory feedback for the patient. This paper presents two sonification approaches in medicine: a balancing coordination system and a robot for moving the legs after serious injuries of the lower body parts. These two systems are evaluated and compared based on the method of sonification, and transmission and analysis of the auditory information. Finally, a supposed method for using musical notes and measures is presented, and a selection method for the length of sonification based on the initial time interval is suggested.</t>
+  </si>
+  <si>
+    <t>Lukasik, Ewa; Materski, Michal</t>
+  </si>
+  <si>
+    <t>Sonification Of A Virtual Model Of The Old Rare Musical Instrument</t>
+  </si>
+  <si>
+    <t>The paper describes a project whose goal was to enable users realistically interact with a 3D virtual model of a historical musical instrument – the clavichord attributed to the famous 18th century maker. A challenge of enabling the user to play the virtual copy of the instrument was resolved by using the dynamic MIDI keyboard. The prerecorded clavichord sound samples are controlled by the software using the MIDI commands. Playing the real keyboard is synchronized with the movement of virtual keys and other parts of sound generating mechanism. The sound effects, characteristic for the clavichord Tragen der Tonne and Bebung may be imitated, which gives the user the impression of playing the real instrument.</t>
+  </si>
+  <si>
+    <t>Landry, Steven; Jeon, Myounghoon</t>
+  </si>
+  <si>
+    <t>Participatory Design Research Methodologies: A Case Study in Dancer Sonification</t>
+  </si>
+  <si>
+    <t>Given that embodied interaction is widespread in Human-Computer Interaction, interests on the importance of body movements and emotions are gradually increasing. The present paper describes our process of designing and testing a dancer sonification system using a participatory design research methodology. The end goal of the dancer sonification project is to have dancers generate aesthetically pleasing music in real-time based on their dance gestures, instead of dancing to pre-recorded music. The generated music should reflect both the kinetic activities and affective contents of the dancer’s movement. To accomplish these goals, expert dancers and musicians were recruited as domain experts in affective gesture and auditory communication. Much of the dancer sonification literature focuses exclusively on describing the final performance piece or the techniques used to process motion data into auditory control parameters. This paper focuses on the methods we used to identify, select, and test the most appropriate motion to sound mappings for a dancer sonification system.</t>
+  </si>
+  <si>
+    <t>Chafe, Chris; Leistikow, Randal</t>
+  </si>
+  <si>
+    <t>Levels of temporal resolution in sonification of network performance</t>
+  </si>
+  <si>
+    <t>The standard “ping” utility provides a momentary measurement of round trip time. Sequences of ping events are used to gather longer-term statistics about jitter and packet loss in order to describe the quality of service of a network path. A more finegrained tool is needed to evaluate paths which carry interactive media streams for collaborative environments. Natural interaction depends on obtaining consistent low-latency, low-jitter service, something which normally requires several ping “takes” to assess and even then only provides an averaged picture of quality of service. We have designed a stream-based method which directly displays the critical qualities to the ear by continuously driving a bidirectional connection to create sound waves. The network path itself becomes the acoustic medium which our probe sets into vibration. The granularity of this display better matches the time-scales of variance that are important in interactive applications (for example, bidirectional audio streams for long-distance musical collaboration or high-quality teleconference applications). The ear's acuity for pitch fluctuation and timbral constancy make this an unforgiving test. A related sonification technique is discussed which is a sonarlike mapping of momentary ping data to musical tones. Temporal levels of musical foreground, middleground and background can be heard in the melodies derived from the data and correspond to structures that are of importance in the analysis of network performance.</t>
+  </si>
+  <si>
+    <t>Winters, R. Michael; Cumming, Julie E.</t>
+  </si>
+  <si>
+    <t>Sonification of Symbolic Music in the Elvis Project</t>
+  </si>
+  <si>
+    <t>This paper presents the development of sonification in the ELVIS project, a collaboration in interdisciplinary musicology targeting large databases of symbolic music and tools for their systematic analysis. An sonification interface was created to rapidly explore and analyze collections of musical intervals originating from various composers, genres, and styles. The interface visually displays imported musical data as a sound-file, and maps data events to individual short, discrete pitches or intervals. The user can interact with the data by visually zoom in, making selections, playing through the data at various speeds, and adjusting the transposition and frequency spread of the pitches to maximize acoustic comfort and clarity. A study is presented in which rapid pitchmapping is applied to compare differences between similar corpora. A group of 11 participants were able to correctly order collections of sonifications for three composers (Monteverdi, Bach, and Beethoven) and three presentation speeds (10², 10³, and 10⁴ notes/second). Benefits of sonification are discussed including the ability to quickly differentiate composers, find non-obvious patterns in the data, and ‘direct mapping’. The interface is made available as a MacOSX standalone application written in Super- Collider.</t>
+  </si>
+  <si>
+    <t>Barra, Maria; Cillo, Tania; de Santis, Antonio; Petrillo, Umberto Ferraro; Negro, Alberto; Scarano, Vittoro; Matlock, Teenie; Maglio, Paul P.</t>
+  </si>
+  <si>
+    <t>Personal webmelody: Customized sonification of web servers</t>
+  </si>
+  <si>
+    <t>This paper presents Personal WebMelody, a sonified web server that informs its administrator of both normal and abnormal operation through background music. It allows customization and full integration of system-generated music representing web server activity with external music sources (audio CD, MP3, etc) selected by the administrator. Our sonification technique works by associating MIDI or WAV sound tracks with web server events. In an attempt to enable the webmaster to listen to such system-generated music for a long period without becoming fatigued, we introduce the opportunity of mixing an external music source with systemgenerated music. In this way, the administrator can hear the status of the web server while listening to his or her preferred music. We present an empirical study that shows how our web server sonification can convey useful information efficiently.</t>
+  </si>
+  <si>
+    <t>Coop, Allan D.</t>
+  </si>
+  <si>
+    <t>Sonification, Musification, and Synthesis of Absolute Program Music</t>
+  </si>
+  <si>
+    <t>When understood as a communication system, a musical work can be interpreted as data existing within three domains. In this interpretation an absolute domain is interposed as a communication channel between two programatic domains that act respectively as source and receiver. As a source, a programatic domain creates, evolves, organizes, and represents a musical work. When acting as a receiver it re-constitutes acoustic signals into unique auditory experience. The absolute domain transmits physical vibrations ranging from the stochastic structures of noise to the periodic waveforms of organized sound. Analysis of acoustic signals suggest recognition as a musical work requires signal periodicity to exceed some minimum. A methodological framework that satisfies recent definitions of sonification is outlined. This framework is proposed to extend to musification through incorporation of data features that represent more traditional elements of a musical work such as melody, harmony, and rhythm.</t>
+  </si>
+  <si>
+    <t>Ciardi, F. C.</t>
+  </si>
+  <si>
+    <t>sMax: A multimodal toolkit for stock market data sonification</t>
+  </si>
+  <si>
+    <t>In this work, we present sMax a multimodal toolkit for stock market data sonification. Unlike most research focusing their effort primarily on the sonification of single stock information, sMax provides an auditory display for the user to monitor parallel distributed data. sMax uses a set of Java and Max modules to map real time stock market information into recognizable musical patterns. One of the main design goals of the toolkit is to allow low-latency controls over real-time data sonification. Because of its object-oriented architecture, sMax can be easily extended by the user when additional functionality is required. The project outcomes range from the creation of art installations to auditory display for mobile computing devices. We present the theoretical background, and the structure of the program.</t>
+  </si>
+  <si>
+    <t>Sonification: A Prehistory</t>
+  </si>
+  <si>
+    <t>Beilharz, Kirsty; Ferguson, Sam</t>
+  </si>
+  <si>
+    <t>An interface and framework design for interactive aesthetic sonification</t>
+  </si>
+  <si>
+    <t>This paper describes the interface design of our AeSon (Aesthetic Sonification) Toolkit motivated by user-centred customisation of the aesthetic representation and scope of the data. The interface design is developed from 3 premises that distinguish our approach from more ubiquitous sonification methodologies. Firstly, we prioritise interaction both from the perspective of changing scale, scope and presentation of the data and the user's ability to reconfigure spatial panning, modality, pitch distribution, critical thresholds and granularity of data examined. The user, for the majority of parameters, determines their own listening experience for real-time data sonification, even to the extent that the interface can be used for live data-driven performance, as well as traditional information analysis and examination. Secondly, we have explored the theories of Tufte, Fry and other visualization and information design experts to find ways in which principles that are successful in the field of information visualization may be translated to the domain of sonification. Thirdly, we prioritise aesthetic variables and controls in the interface, derived from musical practice, aesthetics in information design and responses to experimental user evaluations to inform the design of the sounds and display. In addition to using notions of meter, beat, key or modality and emphasis drawn from music, we draw on our experiments that evaluated the effects of spatial separation in multivariate data presentations.</t>
+  </si>
+  <si>
+    <t>Seica, Mariana; Martins, Pedro; Roque, Licinio; Cardoso, F. Amilcar</t>
+  </si>
+  <si>
+    <t>A sonification experience to portray the sounds of portuguese consumption habits</t>
+  </si>
+  <si>
+    <r>
+      <t>The stimuli for consumption is present in everyday life, where major retail companies play a role in providing a large range of products every single day. Using sonification techniques, we present a listening experiment of Portuguese consumption habits in the course of ten days, gathered from a Portuguese retail company. We focused on how to represent this time-series data as a musical piece that would engage the listener</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>s attention and promote an active listening attitude, exploring the influence of aesthetics in the perception of auditory displays. Through a phenomenological approach, ten participants were interviewed to gather perceptions evoked by the piece, and how the consumption variations were understood. The tested composition revealed relevant associations about the data, with the consumption context indirectly present throughout the emerging themes: from the idea of everyday life, routine and consumption peaks to aesthetic aspects as the passage of time, frenzy and consumerism. Documentary, movie imagery and soundtrack were also perceived. Several musical aspects were also mentioned, as the constant, steady rhythm and the repetitive nature of the composition, and sensations such as pleasantness, satisfaction, annoyance, boredom and anxiety. These collected topics convey the incessant feeling and consumption needs which portray our present society, offering new paths for comprehending musical sound perception and consequent exploration.</t>
+    </r>
+  </si>
+  <si>
+    <t>Nguyen, Vinh Xuan</t>
+  </si>
+  <si>
+    <t>Tonal DisCo: Dissonance and Consonance in a Gaming Engine</t>
+  </si>
+  <si>
+    <t>Whilst there are several existing toolkits specifically designed for sonification, there has been little investigation into the utilization of computer game engines for sonification. This paper will demonstrate the implementation of a real time game engine for the purpose of sonification and discuss the opportunities and limitations. An important aspect which is lacking in existing sonification toolkits is the ability to sonify streaming data in real-time. Gaming engines not only offer the potential to do this but also offer the ability to visualize data in 3D and in real-time. The sound design of an art exhibition is used as a case study to demonstrate the potential of a computer game editor/sandbox used for visualization and sonification. For the exhibition real-world objects were tracked inside a gallery space and represented in the virtual environment of a computer game, which was displayed on a projector screen. Their movement was sonified into musical form to convey their steady/consistent movement as consonant and their agitated/inconsistent movement as dissonant. Tonal “DisCo” is used to describe their dissonance and consonance rating in both musical tone and visual color. Although the sonification of data into musical structure distorts the accuracy of absolute data values, it does maintain the relationship between data values. This loss of resolution is counteracted by an increase in clarity of data relationships. This case study appropriates the single ratio scale of pitch into both an interval scale of tone and an ordinal scale of octaves in order to express interrelationships.</t>
+  </si>
+  <si>
+    <t>Tsuchiya, Takahiko; Freeman, Jason</t>
+  </si>
+  <si>
+    <t>Spectral Parameter Encoding: Towards a Framework for Functional-Aesthetic Sonification</t>
+  </si>
+  <si>
+    <t>Auditory-display research has had a largely unsolved challenge of balancing functional and aesthetic considerations. While functional designs tend to reduce musical expressivity for the fidelity of data, aesthetic or musical sound organization arguably has a potential for representing multi-dimensional or hierarchical data structure with enhanced perceptibility. Existing musical designs, however, generally employ nonlinear or interpretive mappings that hinder the assessment of functionality. The authors propose a framework for designing expressive and complex sonification using small timescale musical hierarchies, such as the harmony and timbral structures, while maintaining data integrity by ensuring a close-to-the-original recovery of the encoded data utilizing descriptive analysis by a machine listener.</t>
+  </si>
+  <si>
+    <t>Bologna, Guido; Deville, Benoit; Pun, Thierry</t>
+  </si>
+  <si>
+    <t>Pairing Colored Socks and Following a Red Serpentine With Sounds of Musical Instruments</t>
+  </si>
+  <si>
+    <t>The See ColOr interface transforms a small portion of a colored video image into sound sources represented by spatialized musical instruments. This interface aims at providing visually impaired people with a capability of perception of the environment. As a first step of this on-going project, the purpose is to verify the hypothesis that it is possible to use sounds from musical instruments to replace color. Compared to state of the art devices, a quality of the See ColOr interface is that it allows the user to receive a feed-back auditory signal from the environment and its colors, promptly. Two experiments based on a head mounted camera have been performed. The first experiment pertaining to object manipulation is based on the pairing of colored socks, while the second experiment is related to outdoor navigation with the goal of following a colored serpentine. The “socks” experiment demonstrated that seven blindfolded individuals were able to accurately match pairs of colored socks. The same participants successfully followed a red serpentine for more than 80 meters.</t>
+  </si>
+  <si>
+    <t>Upson, R.</t>
+  </si>
+  <si>
+    <t>Educational sonification exercises: Pathways for mathematics and musical achievement</t>
+  </si>
+  <si>
+    <t>This paper reports developments in the use of sonifications and sonification software for educational purposes. Adolescent subjects received training in Cartesian graphing over several sessions with sonification software and a sonification-enhanced curriculum. The project attracted students with low linguistic and logical-mathematical capabilities. Students were engaged by musical composition activities, but they remained anxious about traditional mathematics activities. Though students' mathematical abilities improved only slightly according to a traditional mathematical assessment, this project demonstrated the students' increased comfort level with the subject of mathematics and an increased understanding of the concepts within their own set of linguistics.</t>
+  </si>
+  <si>
+    <t>Vogt, Katharina; Pirro, David; Kobenz, Ingo; Höldrich, Robert; Eckel, Gerhard</t>
+  </si>
+  <si>
+    <t>Physiosonic - movement sonification as auditory feedback</t>
+  </si>
+  <si>
+    <t>We detect human body movement interactively via a tracking sys- tem. This data is used to synthesize sound and transform sound files (music or text). A subject triggers and controls sound param- eters with his or her movement within a pre-set range of motion. The resulting acoustic feedback enhances new modalities of per- ception and the awareness of the body movements. It is ideal for application in physiotherapy and other training contexts. The sounds we use depend on the context and aesthetic pref- erences of the subject. On the one hand, metaphorical sounds are used to indicate the leaving of the range of motion or to make un- intended movements aware. On the other hand, sound material like music or speech is played as intuitive means and motivating feedback to address humans. The sound material is transformed in order to indicate deviations from the target movement. With this sonification approach, subjects perceive the sounds they have cho- sen themselves in undistorted playback as long as they perform the training task appropriately. Our main premises are a simple map- ping of movement to sound and common sense metaphors, that both enhance the understanding for the subject.</t>
+  </si>
+  <si>
+    <t>Vogt, Katharina; Goudarzi, Visda; Parncutt, Richard</t>
+  </si>
+  <si>
+    <t>Empirical Aesthetic Evaluation Of Sonifications</t>
+  </si>
+  <si>
+    <t>This paper discusses three experiments on the aesthetic evaluation of different sonifications. The effects of training and understanding of the auditory display on its aesthetic appealing were tested. Results showed no significant effect, but a trend towards less acceptance due to longer exposure to the sounds in general. Furthermore, there might be effects of musical ability and gender that should be further explored.</t>
+  </si>
+  <si>
+    <t>Taylor, Stephen</t>
+  </si>
+  <si>
+    <t>From Program Music to Sonification: Representation and the Evolution of Music and Language</t>
+  </si>
+  <si>
+    <t>Research into the origins of music and language can shed new light on musical representation, including program music and more recent incarnations such as data sonification. Although sonification and program music have different aims—one scientific explication, the other artistic expression—similar techniques, relying on human and animal biology, cognition, and culture, underlie both. Examples include Western composers such as Beethoven and Berlioz, to more recent figures like Messiaen, Stockhausen and Tom Johnson, as well as music theory, semiotics, biology, and data sonifications by myself and others. The common thread connecting these diverse examples is the use of human musicality, in the biomusicological sense, for representation. Links between musicality and representation—dimensions like high/low, long/short, near/far, etc., bridging the real and abstract—can prove useful for researchers, sound designers, and composers.</t>
+  </si>
+  <si>
+    <t>Rönnberg, Niklas; Lowgren, Jonas</t>
+  </si>
+  <si>
+    <t>Traces of modal synergy: studying interactive musical sonification of images in general-audience use</t>
+  </si>
+  <si>
+    <r>
+      <t>Photone is an interactive installation combining color images with musical sonification. The musical expression is generated based on the syntactic (as opposed to semantic) features of an image as it is explored by the user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>s pointing device, intending to catalyze a holistic user experience we refer to as modal synergy where visual and auditory modalities multiply rather than add. We collected and analyzed two months' worth of data from visitors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> interactions with Photone in a public exhibition at a science center. Our results show that a small proportion of visitors engaged in sustained interaction with Photone, as indicated by session times. Among the most deeply engaged visitors, a majority of the interaction was devoted to visually salient objects, i.e., semantic features of the images. However, the data also contains instances of interactive behavior that are best explained by exploration of the syntactic features of an image, and thus may suggest the emergence of modal synergy.</t>
+    </r>
+  </si>
+  <si>
+    <t>Walker, Bruce N.; Mauney, Lisa M.</t>
+  </si>
+  <si>
+    <t>Individual differences, cognitive abilities, and the interpretation of auditory graphs</t>
+  </si>
+  <si>
+    <t>Auditory graphs exploit pattern recognition in the auditory system, but questions remain about the relationship between cognitive abilities, demographics, and sonification interpretation. Subjects completed a magnitude estimation task relating sound dimensions to data dimensions. Subjects also completed a working memory task (2-back task) and a spatial reasoning task (Raven's Progressive Matrices) to assess cognitive abilities. Demographics, such as gender, age, handedness, and musical experience, were also reported and included in the analysis. A stepwise multiple regression analysis was performed to determine the relationship between the independent (cognitive abilities and demographics) and dependent (individual slopes and R-squared values) variables. The regression analysis indicates some support for most of the predictor variables, especially predicting R-squared values. The 2-back task does not seem to contribute significantly to the interpretation of sonifications and auditory graphs. However, Raven's and many of the demographic variables do show predictive value for interpretation of auditory graphs.</t>
+  </si>
+  <si>
+    <t>Falk, Courtney; Dykstra, Josiah</t>
+  </si>
+  <si>
+    <t>Sonification with music for cybersecurity situational awareness</t>
+  </si>
+  <si>
+    <t>Cyber defenders work in stressful, information-rich, and highstakes environments. While other researchers have considered sonification for security operations centers (SOCs), the mappings of network events to sound parameters have produced aesthetically unpleasing results. This paper proposes a novel sonification process for transforming data about computer network traffic into music. The musical cues relate to notable network events in such a way as to minimize the amount of training time a human listener would need in order to make sense of the cues. We demonstrate our technique on a dataset of 708 million authentication events over nine continuous months from an enterprise network. We illustrate a volume-centric approach in relation to the amplitude of the input data, and also a volumetric approach mapping the input data signal into the number of notes played. The resulting music prioritizes aesthetics over bandwidth to balance performance with adoption.</t>
+  </si>
+  <si>
+    <t>Kalonaris, Stefano</t>
+  </si>
+  <si>
+    <t>Tōkyō kion-on: Query-based generative sonification of atmospheric data</t>
+  </si>
+  <si>
+    <t>Amid growing environmental concerns, interactive displays of data constitute an important tool for exploring and understanding the impact of climate change on the planet’s ecosystemic integrity. This paper presents Tokyo kion-on, a query-based sonification model of Tokyo’s air temperature from 1876 to 2021. The system uses a recurrent neural network architecture known as LSTM with attention trained on a small dataset of Japanese melodies and conditioned upon said atmospheric data. After describing the model’s implementation, a brief comparative illustration of the musical results is presented, along with a discussion on how the exposed hyper-parameters can promote active and non-linear exploration of the data.</t>
+  </si>
+  <si>
+    <t>Kantan, Prithvi Ravi; Spaich, Erika G.; Dahl, Sofia</t>
+  </si>
+  <si>
+    <t>A metaphor-based technical framework for musical sonification in movement rehabilitation</t>
+  </si>
+  <si>
+    <t>Interactive sonification has increasingly shown potential as a means of biofeedback to aid motor learning in movement rehabilitation. However, this application domain faces challenges related to the design of meaningful, task-relevant mappings as well as aesthetic qualities of the sonic feedback. A recent mapping design approach is that of using conceptual metaphors based on image schemata and embodied music cognition. In this work, we developed a framework to facilitate the design and real-time exploration of rehabilitation-tailored mappings rooted in a specific set of music-based conceptual metaphors. The outcome was a prototype system integrating wireless inertial measurement, flexible real-time mapping control and physical modelling-based musical sonification. We focus on the technical details of the system, and demonstrate mappings that we created through it for two exercises. These will be iteratively honed and evaluated in upcoming usercentered studies. We believe our framework can be a useful tool in musical sonification design for motor learning applications.</t>
+  </si>
+  <si>
+    <t>Giot, Rudi; Courbe, Yohan</t>
+  </si>
+  <si>
+    <t>InteNtion – Interactive Network Sonification</t>
+  </si>
+  <si>
+    <t>This paper presents an innovative approach in monitoring network traffic by adding a new dimension: the sound. InteNtion (Interactive Network Sonification) is a project aimed at mapping network activity to musical aesthetic. The network traffic analysis is made with the SharpPCap library (a port of WinPCap to C# environment). From this analysis, the collected data are converted into MIDI (Musical Instrument Digital Interface) messages and sent to dedicated synthesizers, which generate sounds dynamically mixed together. The whole process results in an interactive soundscape. This novel approach will initiate two opportunities for technological development. It allows users to actively take part in an interactive exhibition system through simple actions involving network access, including streaming radio over the Internet, sharing music on Twitter, downloading mp3 files and others. This project initiates also a new dimension in monitoring the network by helping the administrator in detecting efficiently the hacking and abuse of the infrastructure.</t>
+  </si>
+  <si>
+    <t>Computational Designing for Auditory Environments</t>
+  </si>
+  <si>
+    <t>This paper is a call for sonification designers to adapt their representational practices from that of designing objects for auditory engagement to the construction of systems of formally described relationships that define the ‘state space’ from which streams of such objects can be drawn. This shift from the crafting individual sonic objects and streams to defining dynamical space of design possibilities we call ‘computational designing’. Such sonification model spaces are inaudible, heard only through its instances, or the manifestations of particular trajectories through the space. Approaching the design of auditory displays as computational tasks poses both considerable challenges and opportunities. These challenges are often understood to be technical, requiring scripting or programming skills, however the main challenge lies in computational design thinking which is not best understood as the extension of established designing processes. The intellectual foundations of computational designing rest at the confluence of multiple fields ranging from mathematics, computer science and systems science to biology, psychophysical and cognitive perception, social science, music theory and philosophy. This paper outlines the fundamental concepts of computational design thinking based on seminal ideas from these fields and explores how they it might be applied to the construction of models for synthesized auditory environments.</t>
+  </si>
+  <si>
+    <t>Yang, Jing; Roth, Andreas</t>
+  </si>
+  <si>
+    <t>Musical features modification for less intrusive delivery of popular notification sounds</t>
+  </si>
+  <si>
+    <t>Less intrusive information delivery has been a popular research topic for auditory displays. While most research has addressed this issue by creating new notification cues such as rendering ambient soundscapes or modifying background music, we present a novel method to gently deliver artificial notification sounds that have been commonly used in digital devices and for popular applications. We propose to play a notification sound by embedding it into the music that a user is listening to, after changing the musical timbre, amplitude, tempo, and octave of the notification to match these features of the music. To implement this concept, we extend a melody extraction algorithm for notification timbre transfer, and we present a pipeline that algorithmically selects a proper time spot and harmoniously embeds the notification into music. To validate our design concept, we present a user study comparing our method with the standard method of playing notification sounds on digital devices. Through an extensive analysis of 96 tasks performed by 32 participants, we demonstrate that our method can deliver notification sounds in a less intrusive but adequately noticeable manner and is preferred by most participants.</t>
+  </si>
+  <si>
+    <t>Schmele, Timothy; Romero, Juan Alzate; Troge, Thomas A.; Ruiter, Nicole; Zapf, Michael</t>
+  </si>
+  <si>
+    <t>Sonifying multichannel ultrasound data for periphonic loudspeaker array</t>
+  </si>
+  <si>
+    <t>The following paper describes several transformations of ultrasonic data into musical material for hemispheric loudspeaker setup. This data comes from a medical prototype for the purpose of early breast cancer detection via 3D multimodal imaging. The data is acquired in a semi-ellipsoid mesh of thousands of ultrasonic emitters and receivers surrounding the measurement object with water as medium. A hemispheric loudspeaker array can reflect this aperture design and offers the possibility of projecting this data in a direct fashion for auditory display. The ultrasounds in the megahertz range are inaudible and need to be transformed into the audible range. We here describe our investigations and methods to transfer medical ultrasound data in an artistic context and report on our insights using different sonification strategies to gain audible, musical material.</t>
+  </si>
+  <si>
+    <t>Snook, Kelly; Barri, Tarik; Goßmann, Joachim; Potts, Jason; Schedel, Margaret; Warm, Hartmut</t>
+  </si>
+  <si>
+    <t>Kepler Concordia: Designing an immersive modular musical and scientific instrument using novel blockchain and sonification technologies in XR</t>
+  </si>
+  <si>
+    <t>This paper describes the first steps in the creation of a new scientific and musical instrument to be released in 2019 for the 400th anniversary of Johannes Kepler's Harmonies of the World, which laid out his three laws of planetary motion and launched the field of modern astronomy. Concordia is a musical instrument that is modularly extensible, with its first software and hardware modules and underlying framework under construction now. The instrument is being designed in an immersive extended-reality (XR) environment with scientifically accurate visualizations and datatransparent sonifications of planetary movements rooted in the musical and mathematical concepts of Johannes Kepler [1], extrapolated into visualizations by Hartmut Warm [2], and sonified. Principles of game design, data sonification/visualization optimization, and digital and analog music synthesis are used in the 3D presentation of information, the user interfaces (UX), and the controls of the instrument, with an optional DIY hardware “cockpit” interface. The instrument hardware and software are both designed to be modular and open source; Concordia can be played virtually without the DIY cockpit on a mobile platform, or users can build or customize their own interfaces, such as traditional keyboards, button grids, or gestural controllers with haptic feedback to interact with the system. It is designed to enable and reward practice and virtuosity through learning levels borrowed from game design, gradually building listening skills for decoding sonified information. The frameworks for uploading, verifying, and accessing the data; programming and verifying hardware and software module builds; tracking of instrument usage; and managing the instrument's economic ecosystem are being built using a combination of distributed computational technologies and peer-to-peer networks, including blockchain and the Interplanetary Filesystem (IPFS). Participants in Concordia fall into three general categories, listed here in decreasing degrees of agency: 1) Contributors; 2) Players; and 3) Observers. This paper lays out the broad structure of Concordia, describes progress on the first software module, and explores the creative, social, economic, and educational potential of Concordia as a new type of creative ecosystem.</t>
+  </si>
+  <si>
+    <t>Orzessek, B.; Falkner, M.</t>
+  </si>
+  <si>
+    <t>Sonification of autonomic rhythms in the frequency spectrum of heart rate variability</t>
+  </si>
+  <si>
+    <t>This poster presents some of the work currently being done at the Paracelsus Clinic in Switzerland on heart rate variability biofeedback with a real time auditory display. Heart rate variability biofeedback is an important diagnostic and therapeutic tool in the work with a wide variety of chronic disorders. We use a proprietary building-block type laboratory computer program that is linked via MIDI to a software sequencer with a VST virtual instrument library. Beyond the sonification of RR intervals as discrete numbers, the development of new techniques became necessary in order to be able to sonify the dynamic, wave-like structure of autonomic rhythms in the frequency spectrum of HRV, what we call ”heartmusic”. The fact that patients can hear their inner autonomic activity as music in real time and so work with elements of their own autonomous rhythmic oscillations, may also add an important new dimension to this field in the future.</t>
+  </si>
+  <si>
+    <t>King, Rob</t>
+  </si>
+  <si>
+    <t>‘Music of the people': Music from data as social commentary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data-music reflects the ubiquity of data in modern society. Composers have not engaged widely with the opportunities opened up by this, despite the chance to overcome a gulf between academic art music and social engagement. Their reluctance might be traced to the challenge of reconciling abstract data and concrete sound, in political implications, and in technological barriers in computer music. The present paper argues that socially relevant music composition for the 21st century can adopt a programme of sonification grounded in politically acute data. As examples of such practice, two compositions are discussed founded upon US and UK social data sets, and realised via the SuperCollider programming language. The consequences for the composer of new music are further discussed from political and musicological angles, with the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾑ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>purpose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of writing such music analysed from the perspective of various commentators.</t>
+    </r>
+  </si>
+  <si>
+    <t>Preliminary guidelines on the sonification of visual artworks: Linking music, sonification &amp; visual arts</t>
+  </si>
+  <si>
+    <t>Sonification and data processing algorithms have advanced over the years to reach practical applications in our everyday life. Similarly, image processing techniques have improved over time. While a number of image sonification methods have already been developed, few have delved into potential synergies through the combined use of multiple data and image processing techniques. Additionally, little has been done on the use of image sonification for artworks, as most research has been focused on the transcription of visual data for people with visual impairments. Our goal is to sonify paintings reflecting their art style and genre to improve the experience of both sighted and visually impaired individuals. To this end, we have designed initial sonifications for paintings of abstractionism and realism, and conducted interviews with visual and auditory experts to improve our mappings. We believe the recommendations and design directions we have received will help develop a multidimensional sonification algorithm that can better transcribe visual art into appropriate music.</t>
+  </si>
+  <si>
+    <t>Childs, E.</t>
+  </si>
+  <si>
+    <t>Achorripsis: A sonification of probability distributions</t>
+  </si>
+  <si>
+    <t>The 1957 musical composition Achorripsis by Iannis Xenakis was composed using four different probability distributions, applied over three different organizational domains, during the course of the 7 minute piece. While Xenakis did not have sonification in mind, his artistic choices in rendering mathematical formulations into musical events (time, space, timbre, glissando speed) provide useful contributions to the “mapping problem” in three significant ways: 1. He pushes the limit of loading the ear with multiple formulations simultaneously. 2. His mapping of “velocity” to string glissando speed provides a useful method of working with a vector quantity with magnitude and direction. 3. His artistic renderings, ie. “musifications” of these distributions, invite the question, in general, as to whether musical/ artistic sonifications are more intelligible to the human ear than sonifications prepared without any musical “filtering” or constraints (e.g. that they could be notated and performed by musicians).</t>
+  </si>
+  <si>
+    <t>England, David; Salces, Fausto J. Sainz; Vickers, Paul</t>
+  </si>
+  <si>
+    <t>Household appliances control device for the elderly</t>
+  </si>
+  <si>
+    <t>An evaluation of musical earcons was carried out to see whether they are an effective and efficient method of delivering information about household appliances to elderly people. A test was carried out to explore the ability of the elderly subjects in remembering and learning the musical earcons. This test indicated a poor rate of recognition of the earcons. A second test that included the presentation of information in three modes (audio, visual and multimodal) was performed to determine which modality was preferred to deliver certain types of information among this group. We hypothesized that the multimodal interface would be the best in terms of speed and accuracy of response, and this was supported by the data. The results showed the need for a redesign of the earcons.</t>
+  </si>
+  <si>
+    <t>Sonification of particle systems via de Broglie's Hypothesis</t>
+  </si>
+  <si>
+    <t>Quantum mechanics states a particle can behave as either a particle or a wave. Thus systems of particles might be likened to a complex superposition of dynamic waves. Motivated by this, the author develops methods for the sonification of particle systems in a logical manner. Many systems and physical phenomena have thus far been simulated, producing a wide range of unique sonic events. The applications that have been explored are for algorithmic sound synthesis and music composition. Of critical importance is addressing the issue of latencies, caused by large complex numerical operations at audio sampling rates. This becomes painfully clear when particles interact with each other. Further applications of this system include scientific sonification, with an appropriate integration of psychoacoustic principles; creating an application for physics and music students to extend and enrich their comprehension of both topics; and inspiring philosophical dialogue regarding the similarities, intersections, and interdependence of Art and Science. Future work aims to produce a real-time application for simulated and real systems, and a deeper integration of quantum mechanics into these techniques.</t>
+  </si>
+  <si>
+    <t>Kikukawa, Yuya; Kato, Megumi; Baba, Tetsuaki; Kushiyama, Kumiko</t>
+  </si>
+  <si>
+    <t>Hakoniwa: A sonification art installation consists of sand and woodblocks</t>
+  </si>
+  <si>
+    <t>In this research we present an interactive tabletop installation ÒHakoniwaÓ. It consists of a wooden box, white sand and painted woodblocks. In this system, corresponding to the arrangement of woodblocks, a ceiling-mounted projector shows visual effects on the sand surface. At the same time, generative music is composed in a computer corresponding to the arrangement of woodblocks and modeling of the sand. This is an attempt of sonification of miniature garden. We studied Sandtray therapy, one of a famous form of art therapy, as a motif of the installation. We directed our attention to tactile sensation of sand and woodblocks, and tried to extend sandtray using computer vision processing and multi-media output. In this paper we describe details of the interactive system and discuss the possibility of supporting primitive play using such interactive systems.</t>
+  </si>
+  <si>
+    <t>Fiedler, Brett L.; Walker, Bruce N.; Moore, Emily B.</t>
+  </si>
+  <si>
+    <t>To sonify or not to sonify? Educator perceptions of auditory display in interactive simulations</t>
+  </si>
+  <si>
+    <t>With the growing presence of auditory display in popular learning tools, it is beneficial to researchers to consider not only the perceptions of the students who use the tools, but the educators who include the tools in their curriculum. We surveyed over 4000 educators to investigate educator perceptions and preferences across four interactive physics simulations for the presence and qualities of non-speech auditory display, as well as surveying users' selfrated musical sophistication as potentially predictive of auditory display preference. We find that the majority of teachers preferred the simulations with auditory display and consistently rated aspects of the experience using simulations with sound positively over the without-sound variants. We also identify simulation design features that align with trends in educator ratings. We did not find the measured musical sophistication to be a predictor of auditory display preference.</t>
+  </si>
+  <si>
+    <t>Zareei, Mo H.; McKinnon, Dugal; Kapur, Ajay; Carnegie, Dale A.</t>
+  </si>
+  <si>
+    <t>Complex: Physical Re-sonification of Urban Noise</t>
+  </si>
+  <si>
+    <t>This paper explores the aesthetic and social values of the noises of modern urban soundscapes and discusses some strategies for boosting the accessibility and appreciation of works of sound art and experimental music that employ them. A proposed audiovisual installation––entitled complex––is outlined as a practical application of techniques designed to reveal the sonic aesthetics of urban technological noise, primarily through resonification and visualization. This will be achieved sonically and physically, by mapping sonic data collected from New York City soundscape (using the Citygram project) onto custom-designed mechatronic soundsculptures.</t>
+  </si>
+  <si>
+    <t>Johannsen, G.</t>
+  </si>
+  <si>
+    <t>Auditory display of directions and states for mobile systems</t>
+  </si>
+  <si>
+    <t>Auditory displays for mobile systems, such as service robots, have been developed. The design of directional sounds and of additional sounds for robot states (e.g., Heavy Load), as well as the design of more complicated robot sound tracks are explained. Basic musical elements and robot movement sounds have been combined. Two experimental studies, on the understandability of the directional sounds and the robot state sounds as well as on the auditory perception of intended robot trajectories in a simulated supermarket scenario, are described. Subjective evaluations of sound characteristics such as urgency, expressiveness, and annoyance have been performed by non-musicians and musicians. These experimental results are compared with the diagrams which have been computed with two wavelet techniques for time-frequency analyses.</t>
+  </si>
+  <si>
+    <t>Khan, Ridwan Ahmed; Jeon, Myounghoon; Yoon, Tejin</t>
+  </si>
+  <si>
+    <t>“Musical Exercise” for people with visual impairments: A preliminary study with the blindfolded</t>
+  </si>
+  <si>
+    <t>Performing independent physical exercise is critical to maintain one's good health, but it is specifically hard for people with visual impairments. To address this problem, we have developed a Musical Exercise platform for people with visual impairments so that they can perform exercise in a good form consistently. We designed six different conditions, including blindfolded or visual without audio conditions, and blindfolded or visual with two different types of audio feedback (continuous vs. discrete) conditions. Eighteen sighted participants participated in the experiment, by doing two exercises - squat and wall sit with all six conditions. The results show that Musical Exercise is a usable exercise assistance system without any adverse effect on exercise completion time or perceived workload. Also, the results show that with a specific sound design (i.e., discrete), participants in the blindfolded condition can do exercise as consistently as participants in the non-blindfolded condition. This implies that not all sounds equally work and thus, care is required to refine auditory displays. Potentials and limitations of Musical Exercise and future works are discussed with the results.</t>
+  </si>
+  <si>
+    <t>Rutz, Hanns Holger; Vogt, Katharina; Höldrich, Robert</t>
+  </si>
+  <si>
+    <t>The SysSon platform: A computer music perspective of sonification</t>
+  </si>
+  <si>
+    <t>We introduce SysSon, a platform for the development and application of sonification. SysSon aims to be an integrative system that serves different types of users, from domain scientists to sonification researchers to composers and sound artists. It therefore has an open nature capable of addressing different usage scenarios. We have used SysSon both in workshops with climatologists and sonification researchers and as the engine to run a real-time sound installation based on climate data. The paper outlines the architecture and design decisions made, showing how a sonification system can be conceived as a collection of specialised abstractions that sit atop a general computer music environment. We report on our experience with SysSon so far and make suggestions about future improvements.</t>
+  </si>
+  <si>
+    <t>Zhang, Ruimin; Barnes, Jaclyn; Ryan, Joseph; Jeon, Myounghoon; Park, Chung Hyuk; Howard, Ayanna M.</t>
+  </si>
+  <si>
+    <t>Musical Robots For Children With ASD Using A Client-Server Architecture</t>
+  </si>
+  <si>
+    <t>People with Autistic Spectrum Disorders (ASD) are known to have difficulty recognizing and expressing emotions, which affects their social integration. Leveraging the recent advances in interactive robot and music therapy approaches, and integrating both, we have designed musical robots that can facilitate social and emotional interactions of children with ASD. Robots communicate with children with ASD while detecting their emotional states and physical activities and then, make real-time sonification based on the interaction data. Given that we envision the use of multiple robots with children, we have adopted a client-server architecture. Each robot and sensing device plays a role as a terminal, while the sonification server processes all the data and generates harmonized sonification. After describing our goals for the use of sonification, we detail the system architecture and on-going research scenarios. We believe that the present paper offers a new perspective on the sonification application for assistive technologies.</t>
+  </si>
+  <si>
+    <t>Newbold, Joseph W.; Bianchi-Berthouze, Nadia; Gold, Nicolas E.</t>
+  </si>
+  <si>
+    <t>Musical Expectancy in Squat Sonification For People Who Struggle With Physical Activity</t>
+  </si>
+  <si>
+    <t>Physical activity is important for a healthy lifestyle. However, it can be hard to stay engaged with exercise and this can often lead to avoidance. Sonification has been used to support physical activity through the optimisation/correction of movement. Though previous work has shown how sonification can improve movement execution and motivation, the specific mechanisms of motivation have yet to be investigated in the context of challenging exercises. We investigate the role of music expectancy as a way to leverage people’s implicit and embodied understanding of music within movement sonification to provide information on technique while also motivating continuation of movement and rewarding its completion. The paper presents two studies showing how this musically informed sonification can be used to support the squat movement. The results show how musical expectancy impacted people’s perception of their own movement, in terms of reward, motivation and movement behaviour and the way in which they moved.</t>
+  </si>
+  <si>
+    <t>A study of exploratory analysis in melodic sonification with structural and durational time scales</t>
+  </si>
+  <si>
+    <t>Melodic sonification is one of the most common methods of sonification: data modulates the pitch of an audio synthesizer over time. This simple sonification, however, still raises questions about how we listen to a melody and perceive the motions and patterns characterized by the underlying data. We argue that analytical listening to such melodies may focus on different ranges of the melody at different times and discover the pitch (and data) relationships gradually over time and after repeated listening. To examine such behaviors in real-time listening to a melodic sonification, we conducted a user study employing interactive time and pitch resolution controls for the user. The study also examines the relationships of these changing time and pitch resolutions to perceived musicality. The results indicate a stronger general relationship between the time progression and the use of time-resolution control to analyze data characteristics, while the pitch resolution controls tend to have more correlation with subjective perceptions of musicality.</t>
+  </si>
+  <si>
+    <t>Roeber, N.; Masuch, M.</t>
+  </si>
+  <si>
+    <t>Interacting with sound: An interaction paradigm for virtual auditory worlds</t>
+  </si>
+  <si>
+    <t>The visual and the auditory field of perception respond on different input signals from our environment. Thus, interacting with worlds solely trough sound is a very challenging task. This paper discusses methods and techniques for sonification and interaction in virtual auditory worlds. In particular, it describes auditory elements such as speech, sound and music and discusses their application in diverse auditory situations, as well as interaction techniques for assisted sonification. The work is motivated by the development of a framework for the interactive exploration of auditory environments which will be used to evaluate the later discussed techniques. The main focus for the design of this framework is the use in narrative environments for auditory games, but also for general purpose auditory user interfaces and communication processes.</t>
+  </si>
+  <si>
+    <t>Quinn, Marty</t>
+  </si>
+  <si>
+    <t>Research set to music: The climate symphony and other sonifications of ice core, radar, DNA, seismic and solar wind data</t>
+  </si>
+  <si>
+    <t>The Climate Symphony and Other Sonifications of Ice Core, Radar, DNA, Seismic and Solar Wind Data is a one-hour performance/presentation of sonification research by Marty Quinn of Design Rhythmics Sonification Research Lab and BAE Systems. It was presented in November 2000 at the National Science Foundation at the invitation of the Director's Office of Public Affairs and the Office of Polar Programs and was warmly received. This paper describes the Climate Symphony portion of the presentation in detail.</t>
+  </si>
+  <si>
+    <t>Coyle, Eugene; Cullen, C.</t>
+  </si>
+  <si>
+    <t>Orchestration within the sonification of basic data sets</t>
+  </si>
+  <si>
+    <t>The use of sonification as a means of representing and analysing data has become a growing field of research in recent years and as such has become a far more accepted means of working with data. Existing work carried out as part of this research has focused primarily on the sonification of DNA/RNA sequences and their subsequent protein structures for the purposes of analysis. This sonification work raised many questions as regards the need for sequences to be set to music in a standard manner so that different strands could be analysed by comparison, and hence the orchestration and instrumentation used became of great importance. The basic principles of sonification can be rapidly extended to include many different data elements within a single rendering, and thus the importance of orchestration grows accordingly. Existing work on the use of rhythmic parsing within a sonification had suggested that far more information could be represented when orchestrated in a rhythmic manner than when simply reconstituted in single musical block. The principle was further extended to include the allocation specific instruments and pitches within rhythmic patterns so that each sonic event would convey the data it was intended to represent. To this end a fictional database of employees in a company was created as a means of developing the principles required for more effective sonification through orchestration. The employee database was intended as a means of using a straightforward data set to analyse the effect of basic changes in instrumentation and orchestration rather than the data itself. The allocation of chord intervals or melodies to different data elements allowed the data to be represented in different ways at output in order that these differences would eventually highlight some form of framework for effective sonification of data sets with multiple elements.</t>
+  </si>
+  <si>
+    <t>Lindborg, PerMagnus; Yuning, David Liu</t>
+  </si>
+  <si>
+    <t>Locust wrath: An iOS audience participatory auditory display</t>
+  </si>
+  <si>
+    <t>Mobile devices have been used in soundscape installations and performances over the past decade or longer, often to emphasize social interaction. Multichannel sonification has been found to successfully represent data describing kinematic phenomena. However, there are few if any examples where these two approaches are combined. The Locust Wrath project has evolved in stages: first, as surround sonifications of climate data for a multimedia dance performance; then, as a frontal display sound installation and as material in a live performance of ‘musical’ interactive sonification; and recently, as an audience participator work. We developed a system for spatialized sonification of data using a server-client model with iOS devices. In two multimedia performances, the audience members’ iPhones were employed ad hoc to constitute a large auditory display. This paper describes the artistic background to the project, outlines the stages, and focuses on the design and implementation of the Locust Wrath client app.</t>
+  </si>
+  <si>
+    <t>Tsuchiya, Takahiko; Freeman, Jason; Lerner, Lee W.</t>
+  </si>
+  <si>
+    <t>Data-to-music API: Real-time data-agnostic sonification with musical structure models</t>
+  </si>
+  <si>
+    <t>In sonification methodologies that aim to represent the underlying data accurately, musical or artistic approaches are often dismissed as being not transparent, likely to distort the data, not generalizable, or not reusable for different data types. Scientific applications for sonification have been, therefore, hesitant to use approaches guided by artistic aesthetics and musical expressivity. All sonifications, however, may have musical effects on listeners, as our trained ears with daily exposure to music tend to naturally distinguish musical and non-musical sound relationships, such as harmony, rhythmic stability, or timbral balance. This study proposes to take advantage of the musical effects of sonification in a systematic manner. Data may be mapped to high-level musical parameters rather than to one-to-one low-level audio parameters. An approach to create models that encapsulate modulatable musical structures is proposed in the context of the new DataTo- Music JavaScript API. The API provides an environment for rapid development of data-agnostic sonification applications in a web browser, with a model-based modular musical structure system. The proposed model system is compared to existing sonification frameworks as well as music theory and composition models. Also, issues regarding the distortion of original data, transparency, and reusability of musical models are discussed.</t>
+  </si>
+  <si>
+    <t>Nees, Michael A.; Harris, Joanna; Leong, Peri</t>
+  </si>
+  <si>
+    <t>How Do People Think They Remember Melodies and Timbres? Phenomenological Reports of Memory for Nonverbal Sounds</t>
+  </si>
+  <si>
+    <t>Memory for nonverbal sounds such as those used in sonifications has been recognized as a priority for cognitiveperceptual research in the field of auditory display. Yet memory processes for nonverbal sounds are not well understood, and existing theory and research have not provided a consensus on a mechanism of memory for nonverbal sounds. We report a new analysis of a qualitative question that asked participants to report the strategy they used to retain nonverbal sounds—both melodies and sounds discriminable primarily by timbre. The question was originally posed as part of the debriefing procedure for three separate memory experiments whose primary findings are reported elsewhere. Results of this new analysis suggested that auditory memory strategies— remembering acoustic properties of sounds—were common across both types of sounds but were more commonly reported for remembering melodies. Motor strategies were also more frequently reported for remembering melodies. Both verbal labeling of sounds and associative strategies—linking the sounds to existing information in memory—were more commonly reported as strategies for remembering sounds discriminable primarily by timbre. Implications for theory and future research are discussed.</t>
+  </si>
+  <si>
+    <t>Multilayered narration in electroacoustic music composition using nuclear magnetic resonance data sonification and acousmatic storytelling</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nuclear magnetic resonance (NMR) spectroscopy is an analytical tool to determine the structure of chemical compounds. Unlike other spectroscopic methods, signals recorded using NMR spectrometers are frequently in a range of zero to 20000 Hz, making direct playback possible. As each type of molecule has, based on its structural features, distinct and predictable features in its NMR spectra, NMR data sonification can be used to create auditory </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾑ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>fingerprints</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of molecules. This paper describes the methodology of NMR data sonification of the nuclei nitrogen, phosphorous, and oxygen and analyses the sonification products of DNA and protein NMR data. The paper introduces On the Extinction of a Species, an acousmatic music composition combining NMR data sonification and voice narration. Ideas developed in electroacoustic composition, such as acousmatic storytelling and sound-based narration are presented and investigated for their use in sonification-based creative works.</t>
+    </r>
+  </si>
+  <si>
+    <t>Spence, Heather Ruth; Ballora, Mark</t>
+  </si>
+  <si>
+    <t>Layers of meaning: The ocean's natural acoustics and the music of its datasets</t>
+  </si>
+  <si>
+    <t>The transdisciplinary National Academies Keck Futures Initiative (NAKFI) conference on the Deep Blue Sea sparked a collaboration between sonification expert Mark Ballora and marine biologist and sound artist Heather Spence. Research involving long-term Marine Passive Acoustic Monitoring (MPAM) of the MesoAmerican Reef system forms the basis for a gradient of audio products: 1) layering a tour guide acoustic instrument over raw and manipulated soundscape recordings; 2) layering of multiple acoustic instruments over duty cycle interpretation sampling; and 3) layering of data sonification over the original data, with additional acoustic instrument layers. The audio products are designed to promote data exploration and understanding by researchers and students, as well as an emotional impact musically with conservation themes. Presentations have included live and virtual performances and workshops. Next steps include sonification of other correlated environmental data with the original sound data in raw, manipulated, and sonified forms.</t>
+  </si>
+  <si>
+    <t>The sonification of numerical fluid flow simulations</t>
+  </si>
+  <si>
+    <t>Computational Fluid Dynamics (CFD) software simulates fluid, air flow and heat transfer by solving the Navier-Stokes (N-S) equations numerically. Realistic 3-D engineering simulations typically yield the values of 7 or more variables (e.g. fluid component velocities and temperatures) at hundreds of thousands of points in space, all as a function of time. It has been noted that solutions of the N-S equations sometimes yield highly complex, non-linear flow fields which can be aesthetically interesting from a purely visual standpoint. The analysis of CFD results may benefit substantially from sonification, to depict convergence behavior, scan large amounts of data with low activity, or codify global events in the flow field. As a corollary to this interest in developing CFD sonification techniques, we can explore its unusual potential as a tool for algorithmic musical composition. This paper will report the results of an initial implementation of the author's port of the two-dimensional, steady, laminar CFD code TEACH-L on a JAVA platform, in which the numerical output is linked in real time to the JSyn digital audio synthesis package. The sonification of steady, laminar, developing flow in a two dimensional duct will be described in detail.</t>
+  </si>
+  <si>
+    <t>Fan, Jianyu; Topel, Spencer</t>
+  </si>
+  <si>
+    <t>SonicTaiji: A Mobile Instrument for Taiji Performance</t>
+  </si>
+  <si>
+    <t>SonicTaiji is a mobile instrument designed for the Android Platform. It utilizes accelerometer detection, sound synthesis, and data communication techniques to achieve real-time Taiji sonification. Taiji is an inner-strength martial art aimed at inducing meditative states. In this mobile music application, Taiji movements are sonified via gesture detection, connecting listening and movement. This instrument is a tool for practitioners to enhance the meditative experience of performing Taiji. We describe the implementation of gesture position selection, real-time synthesis, and data mapping. We describe outcomes of subjective tests of the user experience.</t>
+  </si>
+  <si>
+    <t>Lemmens, Paul M. C.</t>
+  </si>
+  <si>
+    <t>Using the major and minor mode to create affectively-charged earcons</t>
+  </si>
+  <si>
+    <t>The importance of the structured fabrication of auditory (feedback) signals like earcons is common knowledge in the ICAD community. To create such structured families of earcons musical transformations like rhythm or pitch (and many others) are usually employed. However, one important transformation in Western tonal music, that of the distinction between major and minor mode, to our knowledge, has not been exploited, despite the fact that the affective connotation of the major and minor mode might be useful for research into auditory signals for affective human– computer interfaces. The present study investigated whether the transformation to major or minor mode can be used to create affectively–charged earcons for use in affective– computing research [1]. The affective–congruency effect that we obtained provides evidence that the processing of affective information can interfere with making rational, cognitive decisions. We argue that the transformation to the major or minor mode is suitable to create affectively–charged earcons and that it is important to ensure affective correspondence in computer interfaces to be able to realize optimal performance levels.</t>
+  </si>
+  <si>
+    <t>Palomaki, H.</t>
+  </si>
+  <si>
+    <t>Meanings conveyed by simple auditory rhythms</t>
+  </si>
+  <si>
+    <t>In this article we concentrate on perception of non-musical rhythm. The purpose of this study has been to find possible meanings related to simple auditory rhythms. Meanings were examined using semantic scales. 26 subjects rated nine different rhythm samples according to adjective pair scales. We also identify some preliminary design suggestions as to how rhythm can be used in sonification and discuss duration limitation when composing earcons.</t>
+  </si>
+  <si>
+    <t>Sonification Strategies for the Film Rhythms of the Universe</t>
+  </si>
+  <si>
+    <t>Design strategies are discussed for sonifications that were created for the short film Rhythms of the Universe, which was conceived by a cosmologist and a musician, with multi-media contributions from a number of artists and scientists. Sonification functions as an engagement factor in this scientific outreach project, along with narration, music, and visualization. This paper describes how the sonifications were created from datasets describing pulsars, the planetary orbits, gravitational waves, nodal patterns in the sun’s surface, solar winds, extragalactic background light, and cosmic microwave background radiation.</t>
+  </si>
+  <si>
+    <t>Savery, Richard; Ayyagari, Madhukesh; May, Keenan; Walker, Bruce N.</t>
+  </si>
+  <si>
+    <t>Soccer sonification: Enhancing viewer experience</t>
+  </si>
+  <si>
+    <t>We present multiple approaches to soccer sonification, focusing on enhancing the experience for a general audience. For this work, we developed our own soccer data set through computer vision analysis of footage from a tactical overhead camera. This data-set included X, Y, coordinates for the ball and players throughout, as well as passes, steals and goals. After a divergent creation process, we developed four main methods of sports sonification for entertainment. For the Tempo Variation and Pitch Variation methods, tempo or pitch is operationalized to demonstrate ball and player movement data. The Key Moments method features only pass, steal and goal data, while the Musical Moments method takes existing music and attempts to align the track with important data points. Evaluation was done using a combination of qualitative focus groups and quantitative surveys, with 36 participants completing hour long sessions. Results indicated an overall preference for the Pitch Variation and Musical Moments methods, and revealed a robust trade-off between usability and enjoyability.</t>
+  </si>
+  <si>
+    <t>Perez-Lopez, Andres</t>
+  </si>
+  <si>
+    <t>3DJ: A supercollider framework for real-time sound spatialization</t>
+  </si>
+  <si>
+    <t>The field of real time sound spatizalization is recently receiving much attention, as suggested by the large number of proposals appeared in last years - both from software spatialization frameworks and from hardware spatialization interfaces. However, most of the proposed works do not take into account the existing knowledge in Human Computer Interaction Design, which causes them to remain in a simplified approach. We propose a theoretical basis for real-time spatialization design from a holistic perspective, based on the Digital Musical Instruments theory, and use it to provide a comparative review of recent proposals. Furthermore, we develop our own state-of-the-art software spatialization system, 3Dj, which may help in the task of design and evaluation of new proposals for real-time sound spatialization in the fields of interactive performance, data sonification or virtual environments.</t>
+  </si>
+  <si>
+    <t>García Riber, Adrian</t>
+  </si>
+  <si>
+    <t>Sonifigrapher: Sonified light curve synthesizer</t>
+  </si>
+  <si>
+    <r>
+      <t>In an attempt to contribute to the constant feedback existing between science and music, this work describes the design strategies used in the development of the virtual synthesizer prototype called Sonifigrapher. Trying to achieve new ways of creating experimental music through the exploration of exoplanet data sonifications, this software provides an easy-touse graph-to-sound quadraphonic converter, designed for the sonification of the light curves from NASA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ﾒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>s publiclyavailable exoplanet archive. Based on some features of the first analog tape recorder samplers, the prototype allows end-users to load a light curve from the archive and create controlled audio spectra making use of additive synthesis sonification. It is expected to be useful in creative, educational and informational contexts as part of an experimental and interdisciplinary development project for sonification tools, oriented to both non-specialized and specialized audiences.</t>
+    </r>
+  </si>
+  <si>
+    <t>Riber, Adrián García</t>
+  </si>
+  <si>
+    <t>Planethesizer: Approaching exoplanet sonification</t>
+  </si>
+  <si>
+    <t>The creation of simulations, sounds and images based on information related to an object of investigation is currently a real tool used in multiple areas to bring the non-specialized public closer to scientific achievements and discoveries. Under this context of multimodal representations and simulations developed for educational and informational purposes, this work intends to build a bridge between virtual musical instruments’ development and physical models, using the gravitation laws of the seven planets orbiting around the Trappist-1 star. The following is a case study of an interdisciplinary conversion algorithm design that relates musical software synthesis to exoplanets’ astronomical data - measured from the observed flux variations in the light curves of their star- and that tries to suggest a systematic and reproducible method, useful for any other planetary system or model-based virtual instrument design. As a result, the Virtual Interactive Synthesizer prototype Planethesizer is presented, whose default configurations display a multimodal Trappist-1, Kepler-444 and K2-72 planetary systems simulation.</t>
+  </si>
+  <si>
+    <t>Boren, Braxton; Genovese, Andrea</t>
+  </si>
+  <si>
+    <t>Acoustics of virtually coupled performance spaces</t>
+  </si>
+  <si>
+    <t>Many different musical applications, including remote sonification, sound installation, augmented reality, and distributed/ telematic music performance, make use of high speed Internet connections between different performance spaces. Most of the technical literature on this subject focuses on system latency, but there are also significant contributions from the acoustics of all rooms connected: specifically, smaller auxiliary rooms will tend to introduce spectral coloration, and the “main” larger volume will send more reverberation to the off-site performers. Measurements taken in two linked networked sites used in telematic performance show that both of these issues are present. Some improvements are suggested, including physical room alterations and equalization methods using signal processing.</t>
+  </si>
+  <si>
+    <t>Barrett, Natasha; Nymoen, Kristian</t>
+  </si>
+  <si>
+    <t>Investigations in coarticulated performance gestures using interactive parameter-mapping 3D sonification</t>
+  </si>
+  <si>
+    <t>Spatial imagery is one focus of electroacoustic music, more recently advanced by 3D audio furnishing new avenues for exploring spatio-musical structures and addressing what can be called a tangible acousmatic experience. In this paper we present new insights into spatial, temporal and sounding coarticulated (contextually smeared) gestures by applying interactive parameter-mapping sonification in three-dimensional highorder ambisonics, numerical analysis and spatial composition. 3D motion gestures and audio performance data are captured and then explored in sonification. Spatial motion combined with spatial sound is then numerically analyzed to isolate gestural objects and smaller coarticulated atoms in time, space and sound. The results are then used to explore the acousmatic coarticulated image and as building blocks for a composed dataset embodying the original gestural performance. This new data is then interactively sonified in 3D to create acousmatic compositions embodying tangible gestural imagery.</t>
+  </si>
+  <si>
+    <t>Fernstrom, Mikael; McNamara, Caolan</t>
+  </si>
+  <si>
+    <t>After direct manipulation - direct sonification</t>
+  </si>
+  <si>
+    <t>The effectiveness of providing multiple-stream audio to support browsing on a computer was investigated through the iterative development and evaluation of a series of sonic browser prototypes. The data set used was a database containing music. Interactive sonification1 was provided in conjunction with simplified human-computer interaction sequences. It was investigated to what extent interactive sonification with multiple-stream audio could enhance browsing tasks, compared to interactive sonification with single-stream audio support. With ten users it was found that with interactive multiple-stream audio the users could accurately complete the browsing tasks significantly faster than those who had single-stream audio support.</t>
+  </si>
+  <si>
+    <t>McLachlan, Ross; McGee-Lennon, Marilyn; Brewster, Stephen</t>
+  </si>
+  <si>
+    <t>The sound of musicons: investigating the design of musically derived audio cues</t>
+  </si>
+  <si>
+    <t>Musicons (brief samples of well-known music used in auditory interface design) have been shown to be memorable and easy to learn. However, little is known about what actually makes a good Musicon and how they can be created. This paper reports on an empirical user study (N=15) to explore the recognition rate and preference ratings for a set of Musicons that were created by allowing users to self-select 5 second sections from (a) a selection of their own music and (b) a set of control tracks. It was observed that sampling a 0.5 second Musicon from a 5-second musical section resulted in easily identifiable and well liked Musicons. Qualitative analysis highlighted some of the underlying properties of the musical sections that resulted in ‘good’ Musicons. A preliminary set of guidelines is presented that provides a greater understanding of how to create effective and identifiable Musicons for future auditory interfaces.</t>
+  </si>
+  <si>
+    <t>Sturm, B. L.</t>
+  </si>
+  <si>
+    <t>Surf music: Sonification of ocean buoy spectral data</t>
+  </si>
+  <si>
+    <t>The Coastal Data Information Program (CDIP) has been collecting data on ocean wave conditions since late 1975, first using arrays of pressure sensors, and more recently directional buoys. Fourier analysis of the data reveals the spectral and directional content of the wave-driven motions measured by the buoy. Shifting the spectrum to an audible range and synthesizing a time-domain signal creates an aurally interesting and illuminating sonification of ocean wave dynamics. The work done so far has been guided by artistic curiosity; but input from a senior oceanographer has given guidance toward interpretation and elaboration of the methodology. Examples of ocean buoy spectral data sonification are presented, each illustrating important aspects of physical oceanography. Three forms of the data are sonified, from the least detailed to the most. The obvious sonic events are the effects of energy from storms, both local and far away. From the sonification one can estimate the energy of the storm, and the distance it originated. Entire years of data have been sonified in one to thirty minute durations for buoys in different regions, which demonstrate dramatic seasonal and regional differences. Also displayed are the time-lags of South moving storm energies at three distantly separated points on the West Coast of the United States.</t>
+  </si>
+  <si>
+    <t>Mathew, Marlene; Cetinkaya, Mert; Roginska, Agnieszka</t>
+  </si>
+  <si>
+    <t>BSONIQ: A 3-D EEG Sound Installation</t>
+  </si>
+  <si>
+    <t>Brain Computer Interface (BCI) methods have received a lot of attention in the past several decades, owing to the exciting possibility of computer-aided communication with the outside world. Most BCIs allow users to control an external entity such as games, prosthetics, musical output etc. or are used for offline medical diagnosis processing. Most BCIs that provide neurofeedback, usually categorize the brainwaves into mental states for the user to interact with. Raw brainwave interaction by the user is not usually a feature that is readily available for a lot of popular BCIs. If there is, the user has to pay for or go through an additional process for raw brain wave data access and interaction. BSoniq is a multi-channel interactive neurofeedback installation which, allows for real-time sonification and visualization of electroencephalogram (EEG) data. This EEG data provides multivariate information about human brain activity. Here, a multivariate event-based sonification is proposed using 3D spatial location to provide cues about these particular events. With BSoniq, users can listen to the various sounds (raw brain waves) emitted from their brain or parts of their brain and perceive their own brainwave activities in a 3D spatialized surrounding giving them a sense that they are inside their own heads.</t>
+  </si>
+  <si>
+    <t>Cowden, Patrick; Dosiek, Luke</t>
+  </si>
+  <si>
+    <t>Auditory displays of electric power grids</t>
+  </si>
+  <si>
+    <t>This paper presents auditory displays of power grid voltage. Due to the constantly changing energy demands experienced by a power system, the voltage varies slightly about nominal, e.g., 120±2 V at 60±0.04 Hz. These variations are small enough that any audible effects, such as transformer hum, appear to have constant volume and pitch. Here, an audification technique is derived that amplifies the voltage variations and shifts the nominal frequency from 60 Hz to a common musical note. Sonification techniques are presented that map the voltage magnitude and frequency to MIDI velocity and pitch, and create a sampler trigger from frequency deviation. Several examples, including audio samples, are given under a variety of power system conditions. These results culminate in a multi-instrument track generated from the sonification of time-synchronized geographically widespread power grid measurements. In addition, an inexpensive Arduino-based device is detailed that allows for real-time sonification of wall outlet voltage.</t>
+  </si>
+  <si>
+    <t>Sonifyd: A graphical approach for sound synthesis and synesthetic visual expression</t>
+  </si>
+  <si>
+    <t>This paper describes Sonifyd, a sonification driven multimedia and audiovisual environment based on color-sound conversion for real-time manipulation. Sonifyd scans graphics horizontally or vertically from a scan line, generates sound and determines timbre according to its own additive synthesis based color-to-sound mapping. Color and sound relationships are fixed as default, but they can be organic for more tonal flexibility. Within this ecosystem, flexible timbre changes will be discovered by Sonifyd. The scan line is invisible, but Sonifyd provides another display that represents the scanning process in the form of dynamic imagery representation. The primary goal of this project is to be a functioning tool for a new kind of visual music, graphic sonification research and to further provide a synesthetic metaphor for audiences/users in the context of an art installation and audiovisual performance. The later section is a discussion about limitations that I have encountered: using an additive synthesis and frequency modulation technique with the line scanning method. In addition, it discusses potential possibilities for the future direction of development in relation to graphic expression and sound design context.</t>
+  </si>
+  <si>
+    <t>Berger, Jonathan; Wang, Ge; Chang, Mindy</t>
+  </si>
+  <si>
+    <t>Sonification and Visualization of Neural Data</t>
+  </si>
+  <si>
+    <t>This paper describes a method for integrating audio and visual displays to explore the activity of neurons in the brain. The motivation is twofold: to help understand how populations of neurons respond during cognitive tasks and in turn explore how signals from the brain might be used to create musical sounds. Experimental data was drawn from electrophysiological recordings of individual neurons in awake behaving monkeys, and an interface was designed to allow the user to step through a visual task as seen by the monkey along with concurrent sonification and visualization of activity from a population of recorded neurons. Data from two experimental paradigms illustrating different functional properties of neurons in the prefrontal cortex during attention and decisionmaking tasks are presented. The current system provides an accessible way to learn about how neural activity underlies cognitive functions and serves as a preliminary framework to explore both analytical and aesthetic dimensions of audiovisual representations of the data.</t>
+  </si>
+  <si>
+    <t>McGee, Ryan; Rogers, David E.</t>
+  </si>
+  <si>
+    <t>Musification of Seismic Data</t>
+  </si>
+  <si>
+    <t>Seismic events are physical vibrations induced in the earth's crust which follow the general wave equation, making seismic data naturally conducive to audification. Simply increasing the playback rates of seismic recordings and rescaling the amplitude values to match those of digital audio samples (straight audification) can produce eerily realistic door slamming and explosion sounds. While others have produced a plethora of such audifications for international seismic events (i.e. earthquakes), the resulting sounds, while distinct to the trained auditory scientist, often lack enough variety to produce multiple instrumental timbres for the creation of engaging music for the public. This paper discusses approaches of sonification processing towards eventual musification of seismic data, beginning with straight audification and resulting in several musical compositions and new-media installations containing a variety of seismically derived timbres.</t>
+  </si>
+  <si>
+    <t>Back, Maribeth; Des, D.</t>
+  </si>
+  <si>
+    <t>Micro-narratives in sound design: Context, character, and caricature in waveform manipulation</t>
+  </si>
+  <si>
+    <t>This paper reviews sound design techniques used in professional audio for music and theater and proposes a conceptual approach to the construction of audio based in narrative structure. The sound designer does not attempt to replicate "real" sounds; the task is rather to create the impression of a real sound in a listener's mind. In this attempt to create a sound in the listener's mind, the sound designer is aided by user expectations based upon cultural experience as well as physical experience. Practical sound manipulation techniques are discussed in view of their usefulness in matching a listener's mental model of a sound. Narrative aspects of audio design in computational environments are also delineated. Some keywords involved in this paper are sound design, auditory display, multimodal interaction, interface design, narrative, sonic narrative, micro-narrative, and audio.</t>
+  </si>
+  <si>
+    <t>Frid, Emma; Orini, Michele; Martinelli, Giampaolo; Chew, Elaine</t>
+  </si>
+  <si>
+    <t>Mapping inter-cardiovascular time-frequency coherence to harmonic tension in sonification of ensemble interaction between a COVID-19 patient and the medical team</t>
+  </si>
+  <si>
+    <t>This paper presents exploratory work on sonic and visual representations of heartbeats of a COVID-19 patient and a medical team. The aim of this work is to sonify heart signals to reflect how a medical team comes together during a COVID-19 treatment, i.e. to highlight other aspects of the COVID-19 pandemic than those usually portrayed through sonification, which often focuses on the number of cases. The proposed framework highlights synergies between sound and heart signals through mapping between timefrequency coherence (TFC) of heart signals and harmonic tension and dissonance in music. Results from a listening experiment suggested that the proposed mapping between TFC and harmonic tension was successful in terms of communicating low versus high coherence between heart signals, with an overall accuracy of 69%, which was significantly higher than chance. In the light of the performed work, we discuss how links between heart- and sound signals can be further explored through sonification to promote understanding of aspects related to cardiovascular health.</t>
+  </si>
+  <si>
+    <t>Cullen, Charlie; Coyle, Eugene</t>
+  </si>
+  <si>
+    <t>TrioSon: A graphical user interface for pattern sonification</t>
+  </si>
+  <si>
+    <t>The TrioSon software allows users to map musical patterns to input data variables via a graphical user interface (GUI). The application is a Java routine designed to take input files of standard Comma Separated Values (CSV) format and output Standard Midi Files (SMF) using the internal Java Sound API. TrioSon renders output Sonifications from input data files for up to 3 user-defined parameters, allocated as bass, chord and melody instruments for the purposes of arrangement. In this manner each parameter concerned is distinguished by its individual instrumental timbre, with the option of rendering any combination of 1 to 3 parameters as required. The software parses indexed input data relating to individual variables for each user-defined parameter, and provides the means to allocate musical patterns to each variable for Sonification using drag and drop functionality. Control over the Rhythmic Parsing of the Sonification is provided, alongside individual control of the volume, panning, muting and timbre of each instrument in the trio. Sonifications can be rendered as full output files of the entire data, or can also be auditioned by index as required. This feature is designed to allow the user complete control over the data they are sonifying- either on an individual or collective basis. Context for each output Sonification is provided by Midi events defined by the index of the input data, which are mapped to percussive timbres in the final SMF (via track 10). Java development provides the added advantage of portability, with the final application being small enough (200kb) to attach in an email document. It is hoped that the compact and intuitive nature of the application will make it a straightforward means of investigating the Sonification of data sets.</t>
+  </si>
+  <si>
+    <t>Winton, Riley J.; Gable, Thomas M.; Schuett, Jonathan; Walker, Bruce N.</t>
+  </si>
+  <si>
+    <t>A sonification of Kepler space telescope star data</t>
+  </si>
+  <si>
+    <t>A performing artist group interested in including a sonification of star data from NASA’s Kepler space telescope in their next album release approached the Georgia Tech Sonification Lab for assistance in the process. The artists had few constraints for the authors other than wanting the end product to be true to the data, and a musically appealing “heavenly” sound. Several sonifications of the data were created using various techniques, each resulting in a different sounding representation of the Kepler data. The details of this process are discussed in this poster. Ultimately, the researchers were able to produce the desired sounds via sound synthesis, and the artists plan to incorporate them into their next album release.</t>
+  </si>
+  <si>
+    <t>Falkenberg, Kjetil; Frid, Emma; Eriksson, Martin Ljungdahl; Otterbring, Tobias; Daunfeldt, Sven-Olov</t>
+  </si>
+  <si>
+    <t>Auditory notification of customer actions in a virtual retail environment: Sound design, awareness and attention</t>
+  </si>
+  <si>
+    <t>In this paper, we introduce sonification as a less intrusive method for preventing shoplifting. Music and audible alerts are common in retail, and auditory monitoring of a store can aid clerks and reduce losses. Despite these potential advantages, sonification of interaction with goods in retail is an undeveloped field. We conducted an experiment focusing on peripheral auditory notifications in a virtual retail environment, evaluating aspects such as awareness and attention, sound design and noticeability, and localization of event sounds. Results highlighted behavioral differences depending on whether users were informed about the presence of auditory notification sounds or not. The alerts did not cause distraction or annoyance and we suggest that the findings give a promising starting point for future studies and investigations focused on improving the auditory environments in retail.</t>
+  </si>
+  <si>
+    <t>Rouat, Jean; Lescal, Damien; Wood, Sean</t>
+  </si>
+  <si>
+    <t>Handheld Device for Substitution From Vision to Audition</t>
+  </si>
+  <si>
+    <t>Sensorial substitution has great potential in rehabilitation, education, games, and in the creation of music and art. Current technologies allow us to develop sensorial substitution and sonification systems that would not have been imaginable two decades ago. It is desirable to let a large audience use and test sonification systems to provide feedback and improve their design. Handheld devices like smartphones or tablets include network connectivity (WIFI and/or Cellular radio) that can be used to transmit anonymous information about the configuration and strategies adopted by users. It is now feasible to obtain feedback from any user of substitution and sonification technology and not only from a limited number of subjects in the laboratory. Testing in the field with a large number of users is now possible thanks to telecommunication networks and machine learning tools to analyze big data. This work presents a handheld implementation of a simple video sonification system designed to test the acceptability of vision to audition substitution systems and in the near future to provide feedback from users. A first beta version was publicly released in November 2013 as an iOS application for large scale testing. The extended abstract introduces the interface and the underlying technology.</t>
+  </si>
+  <si>
+    <t>Andreopoulou, Areti; Rogińska, Agnieszka; Mohanraj, Hariharan</t>
+  </si>
+  <si>
+    <t>A Database Of Repeated Head-Related Transfer Function Measurements</t>
+  </si>
+  <si>
+    <t>This paper describes a new HRTF collection, measured at the Music and Audio Research Laboratory (MARL), at NYU. This collection of 40 datasets, consists of repeated HRTF measurements on 4 subjects (10 HRTF sets per subject). Analysis of the data offers an understanding of the expected degree of variation in HRTF sets, which, when supported by subjective evaluation, can provide deeper insight for perceptually detected differences between binaural filters. Such knowledge has applications in various research fields and related signal processing tasks, such as: binaural auditory displays, HRTF modeling, and HRTF interpolation.</t>
+  </si>
+  <si>
+    <t>Pun, Thierry; Deville, Benoit; Bologna, Guido</t>
+  </si>
+  <si>
+    <t>Sonification of Colour and Depth in a Mobility Aid for Blind People</t>
+  </si>
+  <si>
+    <t>The See Color interface transforms a small portion of a colored video image into sound sources represented by spatialized musical instruments. Basically, the conversion of colors into sounds is achieved by quantization of the HSL color system. Our purpose is to provide visually impaired individuals with a capability of perception of the environment in real time. In this work the novelty is the simultaneous sonification of color and depth, depth being coded by sound rhythm. Our sonification model is illustrated by several experiments, such as: (1) detecting an open door in order to go out from the office; (2) walking in a hallway and looking for a blue cabinet; (3) walking in a hallway and looking for a red tee shirt; (4) moving outside and avoiding a parked car. Videos with sounds of experiments are available on http://www.youtube.com/guidobologna.</t>
+  </si>
+  <si>
+    <t>Wersényi, György; Répás, József</t>
+  </si>
+  <si>
+    <t>Practical Recommendations For Using Sound Transducers With Glass Memberane As Auditory Display Based On Measurements And Simulations</t>
+  </si>
+  <si>
+    <t>Newly designed vibrating transducers can be used coupled directly to solid surfaces such as wood or glass as plane wave short-distance loudspeakers. Our former analysis evaluated the SolidDrive transducer glued on to glass surfaces of different sizes and forms. Further investigations concluded that these parameters do not influence the transmission and quality of the coupled system significantly. The second part of this investigation included only one size and geometry for further numerical simulations using COMSOL FEM, as well as for acoustic measurements of the transfer function at selected frequencies. Examination of different wall-fixing and mounting methods were also included. Concluding results show that the overall sound quality is inferior to regular loudspeakers, however, using a supplementary subwoofer results in enjoyable music transmission for a short distance. Furthermore, placement of the transducer in the middle of the membrane and having mounting points at the corners are recommended in practical applications</t>
+  </si>
+  <si>
+    <t>Morales, Esteban; James, Kedrick; Horst, Rachel; Takeda, Yuya; Yung, Effiam</t>
+  </si>
+  <si>
+    <t>The sound of our words: Singling, a textual sonification software</t>
+  </si>
+  <si>
+    <t>As visualization struggles to grasp the intricate and temporal networks of meaning found in textual data, sonification emerges as a creative and effective way of representing language. Accordingly, this paper seeks to introduce Singling, a textual sonification software that allows users to create and manipulate auditory representations of a text's lexicogrammatical properties. To achieve this, we first present Singling's main features and interface. We then discuss an example of using this sonification software to explore—both analytically and aesthetically—three different poems. Overall, this paper seeks to introduce researchers, educators, and artists to the many possibilities of Singling and the practice of textual sonification, which includes data analysis, multimodal and collaborative narrative creation, and musical performance to name a few.</t>
+  </si>
+  <si>
+    <t>Shafer, Seth; Larson, Timothy; diFalco, Elaine</t>
+  </si>
+  <si>
+    <t>The sonification of solar harmonics (SOSH) project</t>
+  </si>
+  <si>
+    <t>The Sun is a resonant cavity for very low frequency acoustic waves, and just like a musical instrument, it supports a number of oscillation modes, also commonly known as harmonics. We are able to observe these harmonics by looking at how the Sun's surface oscillates in response to them. Although this data has been studied scientifically for decades, it has only rarely been sonified. The Sonification of Solar Harmonics (SoSH) Project seeks to sonify data related to the field of helioseismology and distribute tools for others to do the same. Creative applications of this research by the authors include musical compositions, installation artwork, a short documentary, and a full-dome planetarium experience.</t>
+  </si>
+  <si>
+    <t>Gygi, Brian; Shafiro, Valeriy</t>
+  </si>
+  <si>
+    <t>From signal to substance and back: Insights from environmental sound research to auditory display design</t>
+  </si>
+  <si>
+    <t>A persistent concern in the field of auditory display design has been how to effectively use environmental sounds, which are naturally occurring familiar non-speech, non-musical sounds. Environmental sounds represent physical events in the everyday world, and thus they have a semantic content that enables learning and recognition. However, unless used appropriately, their functions in auditory displays may cause problems. One of the main considerations in using environmental sounds as auditory icons is how to ensure the identifiability of the sound sources. The identifiability of an auditory icon depends on both the intrinsic acoustic properties of the sound it represents, and on the semantic fit of the sound to its context, i.e., whether the context is one in which the sound naturally occurs or would be unlikely to occur. Relatively recent research has yielded some insights into both of these factors. A second major consideration is how to use the source properties to represent events in the auditory display. This entails parameterizing the environmental sounds so the acoustics will both relate to source properties familiar to the user and convey meaningful new information to the user. Finally, particular considerations come into play when designing auditory displays for special populations, such as hearing impaired listeners who may not have access to all the acoustic information available to a normal hearing listener, or to elderly or other individuals whose cognitive resources may be diminished. Some guidelines for designing displays for these populations will be outlined.</t>
+  </si>
+  <si>
+    <t>Parker, J. no e</t>
+  </si>
+  <si>
+    <t>Sonification as art: Developing praxis for the audification of compost</t>
+  </si>
+  <si>
+    <t>This paper introduces compost as a rich site for creative exploration and expression via the medium of sonification art in the context of Composing [De]Composition, a large-scale audiovisual installation/performance work to be presented at University of California Riverside’s Culver Center for the Arts from June-October 2015. Here, the author non-reductively describes the multiagential and poly-temporal nature of compost through detailing the evolution of an artistic praxis involving: the observation, audification, and sonification of compost temperatures; the development new sensing methods for data-collection; and sound-mapping strategies. The main observable driving the project is incalescence—the heat generated by the composting process. Audification of this biological process brings a perceivably silent activity into the tangible reach of human hearing. The collection and real-time audification of temperature data using a custom interface to route sensor data to MAX/MSP enables listeners to better understand the complex ecology of a heterogeneous mass that is simultaneously decomposing, supporting a myriad of life forms while also enabling the bioavailability of macronutrients to the soil. In addition, the recontexualization of temporally-based temperature data into sound creates fertile ground for exploration in the compositional realm, as the collection of data over time depicts inherent patterns occurring in the systems analyzed, while the basis of music also builds upon the use of patterns (pitch based, rhythmic) through time. Sonification of these patterns enables the composer/sound artist to create compositions in partnership with her subject/phenomenon of study.</t>
+  </si>
+  <si>
+    <t>Davison, Benjamin K.; Walker, Bruce N.</t>
+  </si>
+  <si>
+    <t>Sonification Sandbox Reconstruction: Software Standard for Auditory Graphs</t>
+  </si>
+  <si>
+    <t>We report on an overhaul to the Sonification Sandbox. The Sonification Sandbox provides a cross-platform, flexible tool for converting tabular information into a descriptive auditory graph. It is implemented in Java, using the Java Sound API to generate MIDI output. An improved modular code structure provides a strong user interface and model framework for auditory graph representation and manipulation. A researcher can integrate part or the entire program into a different experimental implementation. The upgraded Sonification Sandbox provides a rich description of the auditory graph representation that can be saved or exported into various file formats. This description includes data representations of pitch, timbre, polarity, pan, and volume, along with graph contexts analogous to visual graph axes. Applications for the Sonification Sandbox include experimentation with various sonification techniques, data analytics beyond visualization, science education, auditory display for the blind, and musical interpretation of data.</t>
+  </si>
+  <si>
+    <t>Hankinson, John CK; Edwards, Alistair DN</t>
+  </si>
+  <si>
+    <t>Musical phrase-structured audio communication</t>
+  </si>
+  <si>
+    <t>It has previously been shown that musical grammars can impose structural constraints upon the design of earcons, thereby providing a grammatical basis to earcon combinations. In this paper, more complex structural combinations are explored, based upon linguistic phrases. By mapping between a musical grammar and a linguistic grammar, musical phrases can be generated which correspond to linguistic sentences. A large number of unique meanings can be presented in this way based upon a simple musical vocabulary. This is of great value to auditory designers. A user study has been undertaken which reveals that users can recognize these complex auditory phrases after a small amount of training.</t>
+  </si>
+  <si>
+    <t>Elmquist, Elias; Ejdbo, Malin; Bock, Alexander; Rönnberg, Niklas</t>
+  </si>
+  <si>
+    <t>OpenSpace sonification: complementing visualization of the solar system with sound</t>
+  </si>
+  <si>
+    <t>Data visualization software is commonly used to explore outer space in a planetarium environment, where the visuals of the software is typically accompanied with a narrator and supplementary background music. By letting sound take a bigger role in these kinds of presentations, a more informative and immersive experience can be achieved. The aim of the present study was to explore how sonification can be used as a complement to the visualization software OpenSpace to convey information about the Solar System, as well as increasing the perceived immersiveness for the audience in a planetarium environment. This was investigated by implementing a sonification that conveyed planetary properties, such as the size and orbital period of a planet, by mapping this data to sonification parameters. With a user-centered approach, the sonification was designed iteratively and evaluated in both an online and planetarium environment. The results of the evaluations show that the participants found the sonification informative and interesting, which suggest that sonification can be beneficially used as a complement to visualization in a planetarium environment.</t>
+  </si>
+  <si>
+    <t>Barri, Tarik; Snook, Kelly</t>
+  </si>
+  <si>
+    <t>Versum: Data Sonification and Visualization in 3D</t>
+  </si>
+  <si>
+    <t>Versum is an advanced, interactive 3D audiovisual composition environment which is augmented with a hardware and software front-end system that maps data into the environment for the purposes of exploratory scientific analysis. Originally intended as an audiovisual sequencer for real-time or automatable music and video performance, Versum also provides a unique environment for systematically investigating new data mappings for optimized human cognition of complex datasets.</t>
+  </si>
+  <si>
+    <t>McGregor, I.; Crerar, A.; Benyon, D.; Macaulay, C.</t>
+  </si>
+  <si>
+    <t>Soundfields and soundscapes: Reifying auditory communities</t>
+  </si>
+  <si>
+    <t>This paper reports progress towards mapping workplace soundscapes. In order to design auditory interfaces that integrate effectively with workplace environments, we need a detailed understanding of the way in which end users inhabit these environments, and in particular, how they interact with the existing auditory environment. Our work concentrates first on mapping the physical soundfield, then overlaying this with a representation of the soundscape as experienced by its active participants. The ultimate aim of this work is to develop an interactive soundscape-mapping tool, analogous to the modeling tools available to architects. Such a tool would be of use to designers of physical, augmented and virtual environments and usable without professional musical or acoustical expertise.</t>
+  </si>
+  <si>
+    <t>Palladino, Dianne K.; Walker, Bruce N.</t>
+  </si>
+  <si>
+    <t>Learning Rates for Auditory Menus Enhanced with Spearcons Versus Earcons</t>
+  </si>
+  <si>
+    <t>Increasing the usability of menus on small electronic devices is essential due to their increasing proliferation and decreasing physical sizes in the marketplace. Auditory menus are being studied as an enhancement to the menus on these devices. This study compared the learning rates for earcons (hierarchical representations of menu locations using musical tones) and spearcons (compressed speech) as potential candidates for auditory menu enhancement. We found that spearcons outperformed earcons significantly in rate of learning. We also found evidence that spearcon comprehension was enhanced by a brief training cycle, and that participants considered the process of learning spearcons much easier than the same process using earcons. Since the efficiency of learning and the perceived ease of use of auditory menus will increase the likelihood they are embraced by those who need them, this paper presents compelling evidence that spearcons may be the superior choice for such applications.</t>
+  </si>
+  <si>
+    <t>Bonebright, Terri L.; Nees, Mike A.; Connerley, Tayla T.; McCain, Glenn R.</t>
+  </si>
+  <si>
+    <t>Testing the effectiveness of sonified graphs for education: A programmatic research project</t>
+  </si>
+  <si>
+    <t>This programmatic research project builds on results from research on data sonification and from studies investigating comprehension of visual graphs. The purpose of the project is to explore the effectiveness of using sonified graphs of real data sets from disciplines to which students are exposed during academic courses. The primary question is whether sonified graphs can increase the comprehension of graphed data for students. The secondary question is whether stereo or monaural sonifications are most effective for graph comprehension. The third and final question of this project is whether sonified graphs with rhythm markers result in better comprehension than sonified graphs without them. The project consists of three laboratory experiments that explore whether students can match auditory representations with the correct visual graphs, whether they can comprehend graphed data sets more effectively by adding sonified components, and whether they can be trained to use sonified graphs better with practice. Results could provide new methods for teaching students with different learning styles quantitative skills in educational settings from kindergarten through college. They could also be extended to assist in teaching students with visual impairments about graphed data sets.</t>
+  </si>
+  <si>
+    <t>Broderick, James; Duggan, Jim; Redfern, Sam</t>
+  </si>
+  <si>
+    <t>Using Auditory Display Techniques to Enhance Decision Making And Perceive Changing Environmental Data Within a 3D Virtual Game Environment</t>
+  </si>
+  <si>
+    <t>When it comes to understanding our environment, we use all our senses. Within the study and implementation of virtual environments and systems, huge advancements in the quality of visuals and graphics have been made, but when it comes to the audio in our environment, many people have been content with very basic sound information. Video games have strived towards powerful sound design, both for player immersion and information perception. Research exists showing how we can use audio sources and waypoints to navigate environments, and how we can perceive information from audio in our surroundings. This research explores using sonification of changing environmental data and environmental objects to improve user's perception of virtual spaces and navigation within simulated environments, with case studies looking at training and for remote operation of unmanned vehicles. This would also expand into how general awareness and perception of dynamic 3D environments can be improved. Our research is done using the Unity3D game engine to create a virtual environment, within which users navigate around water currents represented both visually and through sonification of their information using Csound, a C based programming language for sound and music creation.</t>
+  </si>
+  <si>
+    <t>Sonification of 3D Scenes Using Personalized Spatial Audio to Aid Visually Impaired Persons</t>
+  </si>
+  <si>
+    <t>The research presented concerns the development of a sonification algorithm for representation of 3D scenes for use in an electronic travel aid (ETA) for visually impaired persons. The proposed sonar-like algorithm utilizes segmented 3D scene images, personalized spatial audio and musical sound patterns. The use of segmented and parametrically described 3D scenes allowed to overcome the large sensory mismatch between visual and auditory perception. Utilization of individually measured head related transfer functions (HRTFs), enabled the application of illusions of virtual sound sources. The selection of sounds used was based on surveys with blind volunteers. A number of sonification schemes, dubbed sound codes, were proposed, assigning sound parameters to segmented object parameters. The sonification algorithm was tested in virtual reality using software simulation along with studies of virtual sound source localization accuracy. Afterwards, trials in controlled real environments were made using a portable ETA prototype, with participation of both blind and sighted volunteers. Successful trials demonstrated that it is possible to quickly learn and efficiently use the proposed sonification algorithm to aid spatial orientation and obstacle avoidance.</t>
+  </si>
+  <si>
+    <t>Quinton, Michael; McGregor, Iain; Benyon, David</t>
+  </si>
+  <si>
+    <t>Investigating effective methods of designing sonifications</t>
+  </si>
+  <si>
+    <t>This study aims to provide an insight into effective sonification design. There are currently no standardized design methods, allowing a creative development approach. Sonifcation has been implemented in many different applications from scientific data representation to novel styles of musical expression. This means that methods of practice can vary a greatly. The indistinct line between art and science might be the reason why sonification is still sometimes deemed by scientists with a degree of scepticism. Some well established practitioners argue that it is poor design that renders sonifications meaningless, in-turn having an adverse effect on acceptance. To gain a deeper understanding about sonification research and development 11 practitioners were interviewed. They were asked about methods of sonification design and their insights. The findings present information about sonification research and development, and a variety of views regarding sonification design practice.</t>
+  </si>
+  <si>
+    <t>Reissel, L. M.; Pai, Dinesh K.</t>
+  </si>
+  <si>
+    <t>High-Resolution Analysis and Resynthesis of Environmental Impact Sounds</t>
+  </si>
+  <si>
+    <t>Impact sounds produced by everyday objects are an important source of information about contact interactions in virtual environments and auditory displays. Impact signals also provide a rich class of real and synthetic percussive musical sounds. However, their perceptually acceptable resynthesis and modification requires accurate estimation of mode parameters, which has proved difficult using traditional methods. In this paper we describe some of the problems posed by impact phenomena when applying standard methods, and present a phase-constrained high-resolution algorithm which allows more accurate estimation of modes and amplitudes for impact signals. The phase-constrained algorithm is based on least squares estimation, with initial estimates obtained from a modified ESPRIT algorithm, and it produces better resynthesis results than previously used methods. We give examples with everyday object impact sounds.</t>
+  </si>
+  <si>
+    <t>Lenzi, Sara; Gleria, Francesca</t>
+  </si>
+  <si>
+    <t>Humanising data through sound: Res Extensae and a user-centric approach to data sonification</t>
+  </si>
+  <si>
+    <t>In this paper, starting from a case study (the mixed-media data sonification installation Res Extensae), we discuss a number of assumptions on the efficacy of sound as a means to represent and communicate numerical data. The discussion is supported by the results of a questionnaire aimed at validating our assumptions and conducted with fifteen of the participants to the experience. At the same time, we have the ambition to contribute to a wider debate on the value of data sonification. We introduce the first stage of a research on sonification as a design-driven, user-centred and multi-modal experience, in that closer to data design practices rather than to traditional composition and computer music. We describe the usage of physical objects to help users to put sounds and data into a wider context, improving the user experience and facilitating the comprehension and retention of the meaning of data.</t>
+  </si>
+  <si>
+    <t>Sonification of Movement for Motor Skill Learning in a Novel Bimanual Task: Aesthetics and Retention Strategies</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Here we report early results from an experiment designed to investigate the use of sonification for the learning of a novel perceptual-motor skill. We find that sonification which employs melody is more effective than a strategy which provides only bare timing information. We additionally show that it might be possible to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Grande"/>
+        <family val="2"/>
+      </rPr>
+      <t>�</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>refresh' learning after performance has waned following training - through passive listening to the sound that would be produced by perfect performance. Implications of these findings are discussed in terms of general motor performance enhancement and sonic feedback design.</t>
+    </r>
+  </si>
+  <si>
+    <t>Berman, L. I.; Gallagher, K. B.</t>
+  </si>
+  <si>
+    <t>Listening to program slices</t>
+  </si>
+  <si>
+    <t>Comprehending a computer program can be a daunting task. There is much to understand, including the interaction among different portions of the code. Program slicing can help one to understand this interaction. Because present-day visual development environments tend to become cluttered, the authors have explored sonification of program slices in an attempt to determine if it is practical to offload some of the visual information. Three slice sonification techniques were developed, resulting in an understanding of how to sonify slices in a manner appropriate for the software developer undertaking program comprehension activities. The investigation has also produced a better understanding of sonification techniques that are musical yet non-melodic and non-harmonic. These techniques were demonstrated to a small set of developers, each reporting that the techniques are promising and useful.</t>
+  </si>
+  <si>
+    <t>El Hajj, Tracey</t>
+  </si>
+  <si>
+    <t>Network sonification and the algorhythmics of everyday life</t>
+  </si>
+  <si>
+    <t>Today, public concern with the extent to which they influence people's routines, and how much they affect cultures and societies, has grown substantially. This paper argues that, by listening to networks, people can begin to apprehend, and even comprehend, the complex, ostensibly "magical" nature of network communications. One problem is that listening semantically to networks is incredibly difficult, if not impossible. Networks are very noisy, and they do not, for instance, use alphabetic language for internal or external communication. For the purpose of interpreting networks, I propose "tactical network sonification" (TNS), a technique that focuses on making the materiality of networks sensibly accessible to the general public, especially people who are not technology experts. Using an electromagnetic transduction device — Shintaro Miyazaki and Martin Howse's Detektor — TNS results in crowded sound clips that represent the complexity of network infrastructure, through the many overlapping rhythms and layers of sound that each clip contains.</t>
+  </si>
+  <si>
+    <t>CardioSounds: A portable system to sonify ECG rhythm disturbances in real-time</t>
+  </si>
+  <si>
+    <t>CardioSounds is a portable system that allows users to measure and sonify their electrocardiogram signal in real-time. The ECG signal is acquired using the hardware platform BITalino and subsequently analyzed and sonified using a Raspberry Pi. Users can control basic features from the system (start recording, stop recording) using their smartphone. The system is meant to be used for diagnostic and monitoring of cardiac pathologies, providing users with the possibility to monitor a signal without occupying their visual attention. In this paper, we introduce a novel method, anticipatory mapping, to sonify rhythm disturbances such as Atrial Fibrillation, Atrial flutter and Ventricular Fibrillation. Anticipatory mapping enhances perception of rhythmic details without disrupting the direct perception of the actual heart beat rhythm. We test the method on selected pathological data involving three of the most known rhythm disturbances. A preliminary perception test to assess aesthetics of the sonifications and its possible use in medical scenarios shows that the anticipatory mapping method is regarded as informative discerning healthy and pathological states, however there is no agreement about a preferred sonification type.</t>
+  </si>
+  <si>
+    <t>Hermann, T.; Baier, G.</t>
+  </si>
+  <si>
+    <t>The sonification of rhythms in human electroencephalogram</t>
+  </si>
+  <si>
+    <t>We use sonification of temporal information extracted from scalp EEG to characterize the dynamic properties of rhythms in certain frequency bands. Sonification proves particularly useful in the simultaneous monitoring of several EEG channels. Our results suggest sonification as an important tool in the analysis of multivariate data with subtle correlation differences.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3109,6 +4620,19 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
     <font>
@@ -3139,14 +4663,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3461,16 +4985,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4469A61-734F-2E46-87D8-75D65A40156D}">
-  <dimension ref="A1:G236"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC019B5-D85F-0E4A-8E6C-31B70B34E3DD}">
+  <dimension ref="A1:G388"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="49.1640625" customWidth="1"/>
+    <col min="1" max="7" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -8283,11 +9807,2592 @@
         <v>1013</v>
       </c>
     </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A237" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D237" s="3"/>
+      <c r="E237" s="3"/>
+      <c r="F237" s="3"/>
+      <c r="G237" s="2" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A238" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D238" s="3"/>
+      <c r="E238" s="3"/>
+      <c r="F238" s="3"/>
+      <c r="G238" s="2" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A239" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D239" s="3"/>
+      <c r="E239" s="3"/>
+      <c r="F239" s="3"/>
+      <c r="G239" s="2" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A240" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D240" s="3"/>
+      <c r="E240" s="3"/>
+      <c r="F240" s="3"/>
+      <c r="G240" s="2" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A241" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D241" s="3"/>
+      <c r="E241" s="3"/>
+      <c r="F241" s="3"/>
+      <c r="G241" s="2" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A242" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D242" s="3"/>
+      <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
+      <c r="G242" s="2" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A243" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D243" s="3"/>
+      <c r="E243" s="3"/>
+      <c r="F243" s="3"/>
+      <c r="G243" s="2" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A244" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D244" s="3"/>
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+      <c r="G244" s="2" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A245" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D245" s="3"/>
+      <c r="E245" s="3"/>
+      <c r="F245" s="3"/>
+      <c r="G245" s="2" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A246" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D246" s="3"/>
+      <c r="E246" s="3"/>
+      <c r="F246" s="3"/>
+      <c r="G246" s="2" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A247" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D247" s="3"/>
+      <c r="E247" s="3"/>
+      <c r="F247" s="3"/>
+      <c r="G247" s="2" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A248" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D248" s="3"/>
+      <c r="E248" s="3"/>
+      <c r="F248" s="3"/>
+      <c r="G248" s="2" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A249" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D249" s="3"/>
+      <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+      <c r="G249" s="2" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A250" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D250" s="3"/>
+      <c r="E250" s="3"/>
+      <c r="F250" s="3"/>
+      <c r="G250" s="2" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A251" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D251" s="3"/>
+      <c r="E251" s="3"/>
+      <c r="F251" s="3"/>
+      <c r="G251" s="2" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A252" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D252" s="3"/>
+      <c r="E252" s="3"/>
+      <c r="F252" s="3"/>
+      <c r="G252" s="2" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A253" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D253" s="3"/>
+      <c r="E253" s="3"/>
+      <c r="F253" s="3"/>
+      <c r="G253" s="2" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A254" s="2">
+        <v>1997</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D254" s="3"/>
+      <c r="E254" s="3"/>
+      <c r="F254" s="3"/>
+      <c r="G254" s="2" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A255" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D255" s="3"/>
+      <c r="E255" s="3"/>
+      <c r="F255" s="3"/>
+      <c r="G255" s="3"/>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A256" s="2">
+        <v>1996</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D256" s="3"/>
+      <c r="E256" s="3"/>
+      <c r="F256" s="3"/>
+      <c r="G256" s="2" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A257" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D257" s="3"/>
+      <c r="E257" s="3"/>
+      <c r="F257" s="3"/>
+      <c r="G257" s="2" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A258" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D258" s="3"/>
+      <c r="E258" s="3"/>
+      <c r="F258" s="3"/>
+      <c r="G258" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A259" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D259" s="3"/>
+      <c r="E259" s="3"/>
+      <c r="F259" s="3"/>
+      <c r="G259" s="2" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A260" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D260" s="3"/>
+      <c r="E260" s="3"/>
+      <c r="F260" s="3"/>
+      <c r="G260" s="2" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A261" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D261" s="3"/>
+      <c r="E261" s="3"/>
+      <c r="F261" s="3"/>
+      <c r="G261" s="2" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A262" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D262" s="3"/>
+      <c r="E262" s="3"/>
+      <c r="F262" s="3"/>
+      <c r="G262" s="2" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A263" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D263" s="3"/>
+      <c r="E263" s="3"/>
+      <c r="F263" s="3"/>
+      <c r="G263" s="2" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A264" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D264" s="3"/>
+      <c r="E264" s="3"/>
+      <c r="F264" s="3"/>
+      <c r="G264" s="2" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A265" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D265" s="3"/>
+      <c r="E265" s="3"/>
+      <c r="F265" s="3"/>
+      <c r="G265" s="2" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A266" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D266" s="3"/>
+      <c r="E266" s="3"/>
+      <c r="F266" s="3"/>
+      <c r="G266" s="2" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A267" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D267" s="3"/>
+      <c r="E267" s="3"/>
+      <c r="F267" s="3"/>
+      <c r="G267" s="2" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A268" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D268" s="3"/>
+      <c r="E268" s="3"/>
+      <c r="F268" s="3"/>
+      <c r="G268" s="2" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A269" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D269" s="3"/>
+      <c r="E269" s="3"/>
+      <c r="F269" s="3"/>
+      <c r="G269" s="2" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A270" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D270" s="3"/>
+      <c r="E270" s="3"/>
+      <c r="F270" s="3"/>
+      <c r="G270" s="2" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A271" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D271" s="3"/>
+      <c r="E271" s="3"/>
+      <c r="F271" s="3"/>
+      <c r="G271" s="2" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A272" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D272" s="3"/>
+      <c r="E272" s="3"/>
+      <c r="F272" s="3"/>
+      <c r="G272" s="2" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A273" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D273" s="3"/>
+      <c r="E273" s="3"/>
+      <c r="F273" s="3"/>
+      <c r="G273" s="2" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A274" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D274" s="3"/>
+      <c r="E274" s="3"/>
+      <c r="F274" s="3"/>
+      <c r="G274" s="2" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A275" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D275" s="3"/>
+      <c r="E275" s="3"/>
+      <c r="F275" s="3"/>
+      <c r="G275" s="2" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A276" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D276" s="3"/>
+      <c r="E276" s="3"/>
+      <c r="F276" s="3"/>
+      <c r="G276" s="2" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A277" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D277" s="3"/>
+      <c r="E277" s="3"/>
+      <c r="F277" s="3"/>
+      <c r="G277" s="2" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A278" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D278" s="3"/>
+      <c r="E278" s="3"/>
+      <c r="F278" s="3"/>
+      <c r="G278" s="2" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A279" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D279" s="3"/>
+      <c r="E279" s="3"/>
+      <c r="F279" s="3"/>
+      <c r="G279" s="2" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A280" s="2">
+        <v>1996</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D280" s="3"/>
+      <c r="E280" s="3"/>
+      <c r="F280" s="3"/>
+      <c r="G280" s="2" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A281" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D281" s="3"/>
+      <c r="E281" s="3"/>
+      <c r="F281" s="3"/>
+      <c r="G281" s="2" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A282" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D282" s="3"/>
+      <c r="E282" s="3"/>
+      <c r="F282" s="3"/>
+      <c r="G282" s="2" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A283" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D283" s="3"/>
+      <c r="E283" s="3"/>
+      <c r="F283" s="3"/>
+      <c r="G283" s="2" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A284" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D284" s="3"/>
+      <c r="E284" s="3"/>
+      <c r="F284" s="3"/>
+      <c r="G284" s="2" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A285" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D285" s="3"/>
+      <c r="E285" s="3"/>
+      <c r="F285" s="3"/>
+      <c r="G285" s="2" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A286" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D286" s="3"/>
+      <c r="E286" s="3"/>
+      <c r="F286" s="3"/>
+      <c r="G286" s="2" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A287" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D287" s="3"/>
+      <c r="E287" s="3"/>
+      <c r="F287" s="3"/>
+      <c r="G287" s="2" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A288" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D288" s="3"/>
+      <c r="E288" s="3"/>
+      <c r="F288" s="3"/>
+      <c r="G288" s="2" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A289" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D289" s="3"/>
+      <c r="E289" s="3"/>
+      <c r="F289" s="3"/>
+      <c r="G289" s="2" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A290" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D290" s="3"/>
+      <c r="E290" s="3"/>
+      <c r="F290" s="3"/>
+      <c r="G290" s="2" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A291" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D291" s="3"/>
+      <c r="E291" s="3"/>
+      <c r="F291" s="3"/>
+      <c r="G291" s="2" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A292" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D292" s="3"/>
+      <c r="E292" s="3"/>
+      <c r="F292" s="3"/>
+      <c r="G292" s="2" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A293" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D293" s="3"/>
+      <c r="E293" s="3"/>
+      <c r="F293" s="3"/>
+      <c r="G293" s="2" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A294" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D294" s="3"/>
+      <c r="E294" s="3"/>
+      <c r="F294" s="3"/>
+      <c r="G294" s="2" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A295" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D295" s="3"/>
+      <c r="E295" s="3"/>
+      <c r="F295" s="3"/>
+      <c r="G295" s="2" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A296" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D296" s="3"/>
+      <c r="E296" s="3"/>
+      <c r="F296" s="3"/>
+      <c r="G296" s="2" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A297" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D297" s="3"/>
+      <c r="E297" s="3"/>
+      <c r="F297" s="3"/>
+      <c r="G297" s="3"/>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A298" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D298" s="3"/>
+      <c r="E298" s="3"/>
+      <c r="F298" s="3"/>
+      <c r="G298" s="2" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A299" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D299" s="3"/>
+      <c r="E299" s="3"/>
+      <c r="F299" s="3"/>
+      <c r="G299" s="2" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A300" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D300" s="3"/>
+      <c r="E300" s="3"/>
+      <c r="F300" s="3"/>
+      <c r="G300" s="2" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A301" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D301" s="3"/>
+      <c r="E301" s="3"/>
+      <c r="F301" s="3"/>
+      <c r="G301" s="2" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A302" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D302" s="3"/>
+      <c r="E302" s="3"/>
+      <c r="F302" s="3"/>
+      <c r="G302" s="2" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A303" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D303" s="3"/>
+      <c r="E303" s="3"/>
+      <c r="F303" s="3"/>
+      <c r="G303" s="2" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A304" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D304" s="3"/>
+      <c r="E304" s="3"/>
+      <c r="F304" s="3"/>
+      <c r="G304" s="2" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A305" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D305" s="3"/>
+      <c r="E305" s="3"/>
+      <c r="F305" s="3"/>
+      <c r="G305" s="2" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A306" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D306" s="3"/>
+      <c r="E306" s="3"/>
+      <c r="F306" s="3"/>
+      <c r="G306" s="2" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A307" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D307" s="3"/>
+      <c r="E307" s="3"/>
+      <c r="F307" s="3"/>
+      <c r="G307" s="2" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A308" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D308" s="3"/>
+      <c r="E308" s="3"/>
+      <c r="F308" s="3"/>
+      <c r="G308" s="2" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A309" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D309" s="3"/>
+      <c r="E309" s="3"/>
+      <c r="F309" s="3"/>
+      <c r="G309" s="2" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A310" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D310" s="3"/>
+      <c r="E310" s="3"/>
+      <c r="F310" s="3"/>
+      <c r="G310" s="2" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A311" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D311" s="3"/>
+      <c r="E311" s="3"/>
+      <c r="F311" s="3"/>
+      <c r="G311" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A312" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D312" s="3"/>
+      <c r="E312" s="3"/>
+      <c r="F312" s="3"/>
+      <c r="G312" s="2" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A313" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D313" s="3"/>
+      <c r="E313" s="3"/>
+      <c r="F313" s="3"/>
+      <c r="G313" s="2" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A314" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D314" s="3"/>
+      <c r="E314" s="3"/>
+      <c r="F314" s="3"/>
+      <c r="G314" s="2" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A315" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D315" s="3"/>
+      <c r="E315" s="3"/>
+      <c r="F315" s="3"/>
+      <c r="G315" s="2" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A316" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D316" s="3"/>
+      <c r="E316" s="3"/>
+      <c r="F316" s="3"/>
+      <c r="G316" s="2" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A317" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D317" s="3"/>
+      <c r="E317" s="3"/>
+      <c r="F317" s="3"/>
+      <c r="G317" s="2" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A318" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D318" s="3"/>
+      <c r="E318" s="3"/>
+      <c r="F318" s="3"/>
+      <c r="G318" s="2" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A319" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D319" s="3"/>
+      <c r="E319" s="3"/>
+      <c r="F319" s="3"/>
+      <c r="G319" s="2" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A320" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D320" s="3"/>
+      <c r="E320" s="3"/>
+      <c r="F320" s="3"/>
+      <c r="G320" s="2" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A321" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D321" s="3"/>
+      <c r="E321" s="3"/>
+      <c r="F321" s="3"/>
+      <c r="G321" s="2" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A322" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D322" s="3"/>
+      <c r="E322" s="3"/>
+      <c r="F322" s="3"/>
+      <c r="G322" s="2" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A323" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D323" s="3"/>
+      <c r="E323" s="3"/>
+      <c r="F323" s="3"/>
+      <c r="G323" s="2" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A324" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D324" s="3"/>
+      <c r="E324" s="3"/>
+      <c r="F324" s="3"/>
+      <c r="G324" s="2" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A325" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D325" s="3"/>
+      <c r="E325" s="3"/>
+      <c r="F325" s="3"/>
+      <c r="G325" s="2" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A326" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D326" s="3"/>
+      <c r="E326" s="3"/>
+      <c r="F326" s="3"/>
+      <c r="G326" s="2" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A327" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D327" s="3"/>
+      <c r="E327" s="3"/>
+      <c r="F327" s="3"/>
+      <c r="G327" s="2" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A328" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D328" s="3"/>
+      <c r="E328" s="3"/>
+      <c r="F328" s="3"/>
+      <c r="G328" s="2" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A329" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D329" s="3"/>
+      <c r="E329" s="3"/>
+      <c r="F329" s="3"/>
+      <c r="G329" s="2" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A330" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D330" s="3"/>
+      <c r="E330" s="3"/>
+      <c r="F330" s="3"/>
+      <c r="G330" s="2" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A331" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D331" s="3"/>
+      <c r="E331" s="3"/>
+      <c r="F331" s="3"/>
+      <c r="G331" s="2" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A332" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C332" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D332" s="3"/>
+      <c r="E332" s="3"/>
+      <c r="F332" s="3"/>
+      <c r="G332" s="2" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A333" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D333" s="3"/>
+      <c r="E333" s="3"/>
+      <c r="F333" s="3"/>
+      <c r="G333" s="2" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A334" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B334" s="2" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C334" s="2" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D334" s="3"/>
+      <c r="E334" s="3"/>
+      <c r="F334" s="3"/>
+      <c r="G334" s="2" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A335" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D335" s="3"/>
+      <c r="E335" s="3"/>
+      <c r="F335" s="3"/>
+      <c r="G335" s="2" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A336" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C336" s="2" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D336" s="3"/>
+      <c r="E336" s="3"/>
+      <c r="F336" s="3"/>
+      <c r="G336" s="2" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A337" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B337" s="2" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C337" s="2" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D337" s="3"/>
+      <c r="E337" s="3"/>
+      <c r="F337" s="3"/>
+      <c r="G337" s="2" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A338" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C338" s="2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D338" s="3"/>
+      <c r="E338" s="3"/>
+      <c r="F338" s="3"/>
+      <c r="G338" s="2" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A339" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B339" s="2" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C339" s="2" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D339" s="3"/>
+      <c r="E339" s="3"/>
+      <c r="F339" s="3"/>
+      <c r="G339" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A340" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B340" s="2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C340" s="2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D340" s="3"/>
+      <c r="E340" s="3"/>
+      <c r="F340" s="3"/>
+      <c r="G340" s="2" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A341" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B341" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C341" s="2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D341" s="3"/>
+      <c r="E341" s="3"/>
+      <c r="F341" s="3"/>
+      <c r="G341" s="2" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A342" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D342" s="3"/>
+      <c r="E342" s="3"/>
+      <c r="F342" s="3"/>
+      <c r="G342" s="2" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A343" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B343" s="2" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D343" s="3"/>
+      <c r="E343" s="3"/>
+      <c r="F343" s="3"/>
+      <c r="G343" s="2" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A344" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B344" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D344" s="3"/>
+      <c r="E344" s="3"/>
+      <c r="F344" s="3"/>
+      <c r="G344" s="2" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A345" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D345" s="3"/>
+      <c r="E345" s="3"/>
+      <c r="F345" s="3"/>
+      <c r="G345" s="2" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A346" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B346" s="2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C346" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D346" s="3"/>
+      <c r="E346" s="3"/>
+      <c r="F346" s="3"/>
+      <c r="G346" s="2" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A347" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B347" s="2" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D347" s="3"/>
+      <c r="E347" s="3"/>
+      <c r="F347" s="3"/>
+      <c r="G347" s="2" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A348" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B348" s="2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C348" s="2" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D348" s="3"/>
+      <c r="E348" s="3"/>
+      <c r="F348" s="3"/>
+      <c r="G348" s="2" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A349" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B349" s="2" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C349" s="2" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D349" s="3"/>
+      <c r="E349" s="3"/>
+      <c r="F349" s="3"/>
+      <c r="G349" s="2" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A350" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C350" s="2" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D350" s="3"/>
+      <c r="E350" s="3"/>
+      <c r="F350" s="3"/>
+      <c r="G350" s="2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A351" s="2">
+        <v>1998</v>
+      </c>
+      <c r="B351" s="2" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D351" s="3"/>
+      <c r="E351" s="3"/>
+      <c r="F351" s="3"/>
+      <c r="G351" s="2" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A352" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B352" s="2" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D352" s="3"/>
+      <c r="E352" s="3"/>
+      <c r="F352" s="3"/>
+      <c r="G352" s="2" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A353" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B353" s="2" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C353" s="2" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D353" s="3"/>
+      <c r="E353" s="3"/>
+      <c r="F353" s="3"/>
+      <c r="G353" s="2" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A354" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B354" s="2" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C354" s="2" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D354" s="3"/>
+      <c r="E354" s="3"/>
+      <c r="F354" s="3"/>
+      <c r="G354" s="2" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A355" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B355" s="2" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D355" s="3"/>
+      <c r="E355" s="3"/>
+      <c r="F355" s="3"/>
+      <c r="G355" s="2" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A356" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B356" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D356" s="3"/>
+      <c r="E356" s="3"/>
+      <c r="F356" s="3"/>
+      <c r="G356" s="2" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A357" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B357" s="2" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D357" s="3"/>
+      <c r="E357" s="3"/>
+      <c r="F357" s="3"/>
+      <c r="G357" s="2" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A358" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B358" s="2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D358" s="3"/>
+      <c r="E358" s="3"/>
+      <c r="F358" s="3"/>
+      <c r="G358" s="2" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A359" s="2">
+        <v>1996</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D359" s="3"/>
+      <c r="E359" s="3"/>
+      <c r="F359" s="3"/>
+      <c r="G359" s="2" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A360" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B360" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D360" s="3"/>
+      <c r="E360" s="3"/>
+      <c r="F360" s="3"/>
+      <c r="G360" s="2" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A361" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B361" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D361" s="3"/>
+      <c r="E361" s="3"/>
+      <c r="F361" s="3"/>
+      <c r="G361" s="2" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A362" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B362" s="2" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D362" s="3"/>
+      <c r="E362" s="3"/>
+      <c r="F362" s="3"/>
+      <c r="G362" s="2" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A363" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B363" s="2" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D363" s="3"/>
+      <c r="E363" s="3"/>
+      <c r="F363" s="3"/>
+      <c r="G363" s="2" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A364" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B364" s="2" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C364" s="2" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D364" s="3"/>
+      <c r="E364" s="3"/>
+      <c r="F364" s="3"/>
+      <c r="G364" s="2" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A365" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B365" s="2" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D365" s="3"/>
+      <c r="E365" s="3"/>
+      <c r="F365" s="3"/>
+      <c r="G365" s="2" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A366" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B366" s="2" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C366" s="2" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D366" s="3"/>
+      <c r="E366" s="3"/>
+      <c r="F366" s="3"/>
+      <c r="G366" s="4" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A367" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B367" s="2" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D367" s="3"/>
+      <c r="E367" s="3"/>
+      <c r="F367" s="3"/>
+      <c r="G367" s="2" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A368" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D368" s="3"/>
+      <c r="E368" s="3"/>
+      <c r="F368" s="3"/>
+      <c r="G368" s="2" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A369" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D369" s="3"/>
+      <c r="E369" s="3"/>
+      <c r="F369" s="3"/>
+      <c r="G369" s="2" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A370" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D370" s="3"/>
+      <c r="E370" s="3"/>
+      <c r="F370" s="3"/>
+      <c r="G370" s="2" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A371" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D371" s="3"/>
+      <c r="E371" s="3"/>
+      <c r="F371" s="3"/>
+      <c r="G371" s="2" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A372" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>1403</v>
+      </c>
+      <c r="D372" s="3"/>
+      <c r="E372" s="3"/>
+      <c r="F372" s="3"/>
+      <c r="G372" s="2" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A373" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D373" s="3"/>
+      <c r="E373" s="3"/>
+      <c r="F373" s="3"/>
+      <c r="G373" s="2" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A374" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D374" s="3"/>
+      <c r="E374" s="3"/>
+      <c r="F374" s="3"/>
+      <c r="G374" s="2" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A375" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D375" s="3"/>
+      <c r="E375" s="3"/>
+      <c r="F375" s="3"/>
+      <c r="G375" s="2" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A376" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B376" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="D376" s="3"/>
+      <c r="E376" s="3"/>
+      <c r="F376" s="3"/>
+      <c r="G376" s="2" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A377" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B377" s="2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D377" s="3"/>
+      <c r="E377" s="3"/>
+      <c r="F377" s="3"/>
+      <c r="G377" s="2" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A378" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D378" s="3"/>
+      <c r="E378" s="3"/>
+      <c r="F378" s="3"/>
+      <c r="G378" s="2" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A379" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B379" s="2" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D379" s="3"/>
+      <c r="E379" s="3"/>
+      <c r="F379" s="3"/>
+      <c r="G379" s="2" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A380" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B380" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="C380" s="2" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D380" s="3"/>
+      <c r="E380" s="3"/>
+      <c r="F380" s="3"/>
+      <c r="G380" s="2" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A381" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C381" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D381" s="3"/>
+      <c r="E381" s="3"/>
+      <c r="F381" s="3"/>
+      <c r="G381" s="2" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A382" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D382" s="3"/>
+      <c r="E382" s="3"/>
+      <c r="F382" s="3"/>
+      <c r="G382" s="2" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A383" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D383" s="3"/>
+      <c r="E383" s="3"/>
+      <c r="F383" s="3"/>
+      <c r="G383" s="2" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A384" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B384" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D384" s="3"/>
+      <c r="E384" s="3"/>
+      <c r="F384" s="3"/>
+      <c r="G384" s="2" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A385" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C385" s="2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D385" s="3"/>
+      <c r="E385" s="3"/>
+      <c r="F385" s="3"/>
+      <c r="G385" s="2" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A386" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B386" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C386" s="2" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D386" s="3"/>
+      <c r="E386" s="3"/>
+      <c r="F386" s="3"/>
+      <c r="G386" s="2" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A387" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B387" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C387" s="2" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D387" s="3"/>
+      <c r="E387" s="3"/>
+      <c r="F387" s="3"/>
+      <c r="G387" s="2" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A388" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C388" s="2" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D388" s="3"/>
+      <c r="E388" s="3"/>
+      <c r="F388" s="3"/>
+      <c r="G388" s="2" t="s">
+        <v>1449</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G36" r:id="rId1" display="http://www.locusonus.org/sonification/" xr:uid="{E7CADFAB-871E-7243-BC90-25C6E7498D3B}"/>
-    <hyperlink ref="G62" r:id="rId2" display="http://www.musicntwrk.com/" xr:uid="{A3081A7D-8BD4-804A-8F97-50506DF03090}"/>
-    <hyperlink ref="G117" r:id="rId3" display="http://www.i-maestro.org/" xr:uid="{274C4C93-A59A-0946-A47A-C313BE2A34DB}"/>
+    <hyperlink ref="G36" r:id="rId1" display="http://www.locusonus.org/sonification/" xr:uid="{FAEE1BDF-AC02-D04F-9FBE-6490A4C1C502}"/>
+    <hyperlink ref="G62" r:id="rId2" display="http://www.musicntwrk.com/" xr:uid="{AD29FADA-A6E1-EA41-B92F-8B36EFC23361}"/>
+    <hyperlink ref="G117" r:id="rId3" display="http://www.i-maestro.org/" xr:uid="{DED4E731-B91B-1349-9DB9-37C3A589EAAE}"/>
+    <hyperlink ref="G366" r:id="rId4" display="http://www.youtube.com/guidobologna" xr:uid="{C56E502C-8ACD-054E-92C8-E68F60CBA87D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>